<commit_message>
Design a common card layout
</commit_message>
<xml_diff>
--- a/scripts/cards.xlsx
+++ b/scripts/cards.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\navarog\projects\expeditions\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0471DCD9-45E1-40E9-9808-62814075952B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF21F2C3-8B62-4264-A6D0-F41991DF9460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="34350" windowHeight="21705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -45,28 +40,37 @@
     <t>conditions</t>
   </si>
   <si>
+    <t>benefit</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
     <t>meld</t>
   </si>
   <si>
-    <t>benefit</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
     <t>coins</t>
   </si>
   <si>
+    <t>team</t>
+  </si>
+  <si>
     <t>Akiko</t>
   </si>
   <si>
     <t>character</t>
   </si>
   <si>
-    <t>yellow</t>
-  </si>
-  <si>
-    <t>team</t>
+    <t>Gain 1 face-up meteorite OR Solve; if you Solve, gain the core value of all your solved quests.</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Power, Guile</t>
   </si>
   <si>
     <t>Jiro</t>
@@ -78,10 +82,13 @@
     <t>Activate the previous card’s ability OR Vanquish; if this Vanquish removes the location’s final corruption, you may gain the revealed benefit.</t>
   </si>
   <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>Gain 1 face-up meteorite OR Solve; if you Solve, gain the core value of all your solved quests.</t>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Guile</t>
+  </si>
+  <si>
+    <t>Guile, Guile</t>
   </si>
   <si>
     <t>Matthew</t>
@@ -90,7 +97,10 @@
     <t>Gain a yellow worker OR Solve a quest; if you Solve, gain the core value of all your solved quests.</t>
   </si>
   <si>
-    <t>green</t>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Guile, Power</t>
   </si>
   <si>
     <t>Caesar</t>
@@ -105,7 +115,7 @@
     <t>Gain a face-up quest OR Solve; if you Solve, gain the core value of all your solved quests.</t>
   </si>
   <si>
-    <t>red</t>
+    <t>Red</t>
   </si>
   <si>
     <t>Wojtek</t>
@@ -132,6 +142,9 @@
     <t>Gain a green worker OR Solve; if you Solve, gain the core value of all your solved quests.</t>
   </si>
   <si>
+    <t>Power, Power</t>
+  </si>
+  <si>
     <t>Nacht</t>
   </si>
   <si>
@@ -156,18 +169,33 @@
     <t>item</t>
   </si>
   <si>
+    <t>Whenever you gain a worker, also gain [Power].</t>
+  </si>
+  <si>
     <t>Gain a worker</t>
   </si>
   <si>
     <t>Mitz Valve</t>
   </si>
   <si>
+    <t>Whenever you have 10x[Guile], you may decrease your Guile to 3 and gain $3.</t>
+  </si>
+  <si>
+    <t>Gain [Guile]</t>
+  </si>
+  <si>
     <t>Synergy Halo</t>
   </si>
   <si>
+    <t>Whenever you gain at least 2 [Guile] during your turn, also gain [Power].</t>
+  </si>
+  <si>
     <t>Universal Vise</t>
   </si>
   <si>
+    <t>Whenever you Upgrade this or another item, gain $1 and [Power].</t>
+  </si>
+  <si>
     <t>Upgrade</t>
   </si>
   <si>
@@ -207,12 +235,21 @@
     <t>Chaos Grenade</t>
   </si>
   <si>
+    <t>Whenever you Vanquish, flip a coin. If it’s heads, gain $2. Otherwise, gain [Guile].</t>
+  </si>
+  <si>
     <t>Tesla Pistol</t>
   </si>
   <si>
+    <t>Whenever you Vanquish the final corruption from a location, also gain [Power][Guile].</t>
+  </si>
+  <si>
     <t>Aether Mirror</t>
   </si>
   <si>
+    <t>Whenever you Refresh, gain [Power] or [Guile] per refreshed worker.</t>
+  </si>
+  <si>
     <t>AwakenedShard</t>
   </si>
   <si>
@@ -225,27 +262,45 @@
     <t>Amulet of Bravado</t>
   </si>
   <si>
+    <t>Whenever you have 10x [Power], you may decrease your power to 3 to gain $3.</t>
+  </si>
+  <si>
+    <t>Gain [Power]</t>
+  </si>
+  <si>
     <t>Deceptor Crystal</t>
   </si>
   <si>
+    <t>Whenever you Gather, you may pay [Guile] to include a benefit covered by corruption on your location.</t>
+  </si>
+  <si>
     <t>Gather</t>
   </si>
   <si>
     <t>Parasitic Gauntlet</t>
   </si>
   <si>
+    <t>Whenever you gain a card, you may pay [Power][Guile] to gain $1.</t>
+  </si>
+  <si>
     <t>Gain [Card]</t>
   </si>
   <si>
     <t>Aether-Vision Goggles</t>
   </si>
   <si>
+    <t>Whenever you gain a map, you may gain [Guile] and rearrange your location’s corruption.</t>
+  </si>
+  <si>
     <t>Gain [MapToken]</t>
   </si>
   <si>
     <t>Hover Coil</t>
   </si>
   <si>
+    <t>Whenever you Move through an opponent’s location, that player gains [Guile] and you gain $1.</t>
+  </si>
+  <si>
     <t>Move</t>
   </si>
   <si>
@@ -267,13 +322,16 @@
     <t>Recon Drone</t>
   </si>
   <si>
+    <t>Whenever you Move, you may first either peek at a location within range or gain [Power].</t>
+  </si>
+  <si>
     <t>Flex Capacitor</t>
   </si>
   <si>
     <t>Once per turn, if you discard another card, either gain its core value or activate its ability.</t>
   </si>
   <si>
-    <t>purple</t>
+    <t>Purple</t>
   </si>
   <si>
     <t>Discard [Card]</t>
@@ -301,69 +359,6 @@
   </si>
   <si>
     <t>Fusion Link</t>
-  </si>
-  <si>
-    <t>Power</t>
-  </si>
-  <si>
-    <t>Power, Power</t>
-  </si>
-  <si>
-    <t>Whenever you gain a worker, also gain [Power].</t>
-  </si>
-  <si>
-    <t>Whenever you Upgrade this or another item, gain $1 and [Power].</t>
-  </si>
-  <si>
-    <t>Gain [Power]</t>
-  </si>
-  <si>
-    <t>Whenever you Move, you may first either peek at a location within range or gain [Power].</t>
-  </si>
-  <si>
-    <t>Whenever you have 10x [Power], you may decrease your power to 3 to gain $3.</t>
-  </si>
-  <si>
-    <t>Power, Guile</t>
-  </si>
-  <si>
-    <t>Guile</t>
-  </si>
-  <si>
-    <t>Guile, Guile</t>
-  </si>
-  <si>
-    <t>Guile, Power</t>
-  </si>
-  <si>
-    <t>Whenever you have 10x[Guile], you may decrease your Guile to 3 and gain $3.</t>
-  </si>
-  <si>
-    <t>Gain [Guile]</t>
-  </si>
-  <si>
-    <t>Whenever you gain at least 2 [Guile] during your turn, also gain [Power].</t>
-  </si>
-  <si>
-    <t>Whenever you Vanquish, flip a coin. If it’s heads, gain $2. Otherwise, gain [Guile].</t>
-  </si>
-  <si>
-    <t>Whenever you Vanquish the final corruption from a location, also gain [Power][Guile].</t>
-  </si>
-  <si>
-    <t>Whenever you Refresh, gain [Power] or [Guile] per refreshed worker.</t>
-  </si>
-  <si>
-    <t>Whenever you Gather, you may pay [Guile] to include a benefit covered by corruption on your location.</t>
-  </si>
-  <si>
-    <t>Whenever you gain a card, you may pay [Power][Guile] to gain $1.</t>
-  </si>
-  <si>
-    <t>Whenever you gain a map, you may gain [Guile] and rearrange your location’s corruption.</t>
-  </si>
-  <si>
-    <t>Whenever you Move through an opponent’s location, that player gains [Guile] and you gain $1.</t>
   </si>
   <si>
     <t>Whenever you gain at least 2 [Power] during your turn, also gain [Guile].</t>
@@ -949,13 +944,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -966,12 +966,25 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -980,15 +993,58 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1001,22 +1057,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD675458-7EBB-4B3C-805E-C566CD4A8B20}" name="Table1" displayName="Table1" ref="A1:K103" totalsRowShown="0">
-  <autoFilter ref="A1:K103" xr:uid="{BD675458-7EBB-4B3C-805E-C566CD4A8B20}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F42030B-66C5-46F6-8CFB-CD633B482508}" name="Table1" displayName="Table1" ref="A1:K103" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:K103" xr:uid="{0F42030B-66C5-46F6-8CFB-CD633B482508}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{58EF517F-5EB3-47D1-89E4-0DB6253105A3}" name="name"/>
-    <tableColumn id="2" xr3:uid="{07432D47-7CA4-4F80-82C0-08C652F99B32}" name="type"/>
-    <tableColumn id="3" xr3:uid="{AF485692-B2BC-445E-A554-DC7CD003DBD4}" name="ability"/>
-    <tableColumn id="4" xr3:uid="{83384766-6CAE-416B-9289-10620260E352}" name="worker"/>
-    <tableColumn id="5" xr3:uid="{5CC28BCE-3D7A-4760-B08D-E3DC4B02949C}" name="core"/>
-    <tableColumn id="6" xr3:uid="{F4401A42-F958-441B-9013-F06CD96AC4B9}" name="conditions"/>
-    <tableColumn id="7" xr3:uid="{1EE1E27D-659C-4B6F-B8C5-2DF5E36E848A}" name="benefit"/>
-    <tableColumn id="8" xr3:uid="{0735E75D-633E-410C-9D12-3622AE691CE3}" name="location"/>
-    <tableColumn id="9" xr3:uid="{127880CF-ADEC-46A7-9BA7-3EDE470DE996}" name="meld"/>
-    <tableColumn id="10" xr3:uid="{8FF2DA3F-D507-4E48-8CDC-42230DA60A11}" name="coins"/>
-    <tableColumn id="11" xr3:uid="{0B39E5BA-CCD5-46AD-BE3F-33DAFB19D1D5}" name="team"/>
+    <tableColumn id="1" xr3:uid="{C2006D74-3131-4AFC-AB17-9A5A423535C3}" name="name"/>
+    <tableColumn id="2" xr3:uid="{3C4235A7-DBEF-42F6-B2B8-B558B520A439}" name="type"/>
+    <tableColumn id="3" xr3:uid="{9445079D-106C-44A3-BE10-AD4E28465146}" name="ability"/>
+    <tableColumn id="4" xr3:uid="{5932CE30-2C80-4DE9-AE77-3ED8B40F6703}" name="worker"/>
+    <tableColumn id="5" xr3:uid="{A4D591E4-EA52-4891-94EC-1C91A34809A1}" name="core"/>
+    <tableColumn id="6" xr3:uid="{9C7A2CA8-7EB7-4DB9-9392-D8F07E2B2A42}" name="conditions"/>
+    <tableColumn id="7" xr3:uid="{B031DC88-6162-417C-AEAF-64E92A066380}" name="benefit"/>
+    <tableColumn id="8" xr3:uid="{38F29CF6-B219-4782-8B95-4D953E7749F9}" name="location"/>
+    <tableColumn id="9" xr3:uid="{0C1DFD4D-6D58-4BBF-9103-96680EC6E963}" name="meld"/>
+    <tableColumn id="10" xr3:uid="{8BEE43DE-239D-482B-81BD-AA9B82DCD4C1}" name="coins"/>
+    <tableColumn id="11" xr3:uid="{551EE5F0-3D63-4829-8E14-8064AD20AE34}" name="team"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1031,44 +1087,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1095,15 +1151,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1130,7 +1185,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1142,142 +1196,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -1285,76 +1363,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="I103" sqref="I103"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="1" max="1" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="128.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="141.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>13</v>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -1362,22 +1442,22 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -1385,22 +1465,22 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="K4">
         <v>2</v>
@@ -1408,22 +1488,22 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="K5">
         <v>2</v>
@@ -1431,22 +1511,22 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="K6">
         <v>3</v>
@@ -1454,22 +1534,22 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="K7">
         <v>3</v>
@@ -1477,22 +1557,22 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="K8">
         <v>4</v>
@@ -1500,22 +1580,22 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
       <c r="E9" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="K9">
         <v>4</v>
@@ -1523,22 +1603,22 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="K10">
         <v>5</v>
@@ -1546,22 +1626,22 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="K11">
         <v>5</v>
@@ -1569,22 +1649,22 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="K12">
         <v>6</v>
@@ -1592,22 +1672,22 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="K13">
         <v>6</v>
@@ -1615,22 +1695,22 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>94</v>
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G14" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="J14">
         <v>4</v>
@@ -1638,22 +1718,22 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G15" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="J15">
         <v>2</v>
@@ -1661,22 +1741,22 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G16" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="J16">
         <v>4</v>
@@ -1684,22 +1764,22 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G17" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="J17">
         <v>3</v>
@@ -1707,42 +1787,42 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G18" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="J19">
         <v>4</v>
@@ -1750,22 +1830,22 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="J20">
         <v>2</v>
@@ -1773,22 +1853,22 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="J21">
         <v>3</v>
@@ -1796,22 +1876,22 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G22" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="J22">
         <v>2</v>
@@ -1819,22 +1899,22 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G23" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="J23">
         <v>4</v>
@@ -1842,22 +1922,22 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="J24">
         <v>2</v>
@@ -1865,22 +1945,22 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G25" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="J25">
         <v>2</v>
@@ -1888,22 +1968,22 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G26" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="J26">
         <v>2</v>
@@ -1911,22 +1991,22 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="J27">
         <v>4</v>
@@ -1934,22 +2014,22 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G28" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="J28">
         <v>2</v>
@@ -1957,22 +2037,22 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E29" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G29" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="J29">
         <v>4</v>
@@ -1980,22 +2060,22 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E30" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="J30">
         <v>3</v>
@@ -2003,22 +2083,22 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="D31" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E31" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="J31">
         <v>4</v>
@@ -2026,22 +2106,22 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E32" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G32" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="J32">
         <v>3</v>
@@ -2049,22 +2129,22 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D33" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E33" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G33" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="J33">
         <v>3</v>
@@ -2072,22 +2152,22 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="D34" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E34" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G34" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="J34">
         <v>3</v>
@@ -2095,22 +2175,22 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="D35" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E35" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G35" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="J35">
         <v>2</v>
@@ -2118,22 +2198,22 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" t="s">
         <v>87</v>
-      </c>
-      <c r="D36" t="s">
-        <v>82</v>
-      </c>
-      <c r="E36" t="s">
-        <v>100</v>
-      </c>
-      <c r="G36" t="s">
-        <v>69</v>
       </c>
       <c r="J36">
         <v>2</v>
@@ -2141,22 +2221,22 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="D37" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E37" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G37" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="J37">
         <v>3</v>
@@ -2164,22 +2244,22 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C38" t="s">
         <v>113</v>
       </c>
       <c r="D38" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E38" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G38" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="J38">
         <v>4</v>
@@ -2196,13 +2276,13 @@
         <v>116</v>
       </c>
       <c r="D39" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E39" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F39" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="I39" t="s">
         <v>117</v>
@@ -2219,13 +2299,13 @@
         <v>119</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E40" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F40" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="I40" t="s">
         <v>120</v>
@@ -2242,13 +2322,13 @@
         <v>122</v>
       </c>
       <c r="D41" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E41" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F41" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="I41" t="s">
         <v>123</v>
@@ -2265,13 +2345,13 @@
         <v>125</v>
       </c>
       <c r="D42" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E42" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F42" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="I42" t="s">
         <v>126</v>
@@ -2288,13 +2368,13 @@
         <v>128</v>
       </c>
       <c r="D43" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E43" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F43" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="I43" t="s">
         <v>129</v>
@@ -2311,13 +2391,13 @@
         <v>131</v>
       </c>
       <c r="D44" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E44" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F44" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="I44" t="s">
         <v>132</v>
@@ -2334,13 +2414,13 @@
         <v>134</v>
       </c>
       <c r="D45" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E45" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F45" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="I45" t="s">
         <v>135</v>
@@ -2357,13 +2437,13 @@
         <v>137</v>
       </c>
       <c r="D46" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E46" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F46" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="I46" t="s">
         <v>138</v>
@@ -2380,13 +2460,13 @@
         <v>140</v>
       </c>
       <c r="D47" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E47" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F47" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="I47" t="s">
         <v>141</v>
@@ -2403,13 +2483,13 @@
         <v>143</v>
       </c>
       <c r="D48" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E48" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F48" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="I48" t="s">
         <v>144</v>
@@ -2426,13 +2506,13 @@
         <v>146</v>
       </c>
       <c r="D49" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E49" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F49" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="I49" t="s">
         <v>147</v>
@@ -2449,13 +2529,13 @@
         <v>149</v>
       </c>
       <c r="D50" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E50" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F50" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="I50" t="s">
         <v>150</v>
@@ -2472,13 +2552,13 @@
         <v>152</v>
       </c>
       <c r="D51" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E51" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F51" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="I51" t="s">
         <v>153</v>
@@ -2495,13 +2575,13 @@
         <v>155</v>
       </c>
       <c r="D52" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E52" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F52" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="I52" t="s">
         <v>156</v>
@@ -2518,13 +2598,13 @@
         <v>158</v>
       </c>
       <c r="D53" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E53" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F53" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="I53" t="s">
         <v>159</v>
@@ -2541,13 +2621,13 @@
         <v>161</v>
       </c>
       <c r="D54" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E54" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F54" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="I54" t="s">
         <v>162</v>
@@ -2564,13 +2644,13 @@
         <v>164</v>
       </c>
       <c r="D55" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E55" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F55" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="I55" t="s">
         <v>165</v>
@@ -2587,13 +2667,13 @@
         <v>167</v>
       </c>
       <c r="D56" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E56" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F56" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="I56" t="s">
         <v>168</v>
@@ -2610,13 +2690,13 @@
         <v>170</v>
       </c>
       <c r="D57" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E57" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F57" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="I57" t="s">
         <v>171</v>
@@ -2633,13 +2713,13 @@
         <v>173</v>
       </c>
       <c r="D58" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E58" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F58" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="I58" t="s">
         <v>174</v>
@@ -2656,13 +2736,13 @@
         <v>176</v>
       </c>
       <c r="D59" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E59" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F59" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="I59" t="s">
         <v>177</v>
@@ -2679,13 +2759,13 @@
         <v>179</v>
       </c>
       <c r="D60" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E60" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F60" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="I60" t="s">
         <v>180</v>
@@ -2702,13 +2782,13 @@
         <v>182</v>
       </c>
       <c r="D61" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E61" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F61" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="I61" t="s">
         <v>183</v>
@@ -2725,13 +2805,13 @@
         <v>185</v>
       </c>
       <c r="D62" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E62" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F62" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="I62" t="s">
         <v>186</v>
@@ -2748,13 +2828,13 @@
         <v>188</v>
       </c>
       <c r="D63" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E63" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F63" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="I63" t="s">
         <v>189</v>
@@ -2771,13 +2851,13 @@
         <v>192</v>
       </c>
       <c r="D64" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E64" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F64" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G64" t="s">
         <v>193</v>
@@ -2797,13 +2877,13 @@
         <v>195</v>
       </c>
       <c r="D65" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E65" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F65" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G65" t="s">
         <v>196</v>
@@ -2823,16 +2903,16 @@
         <v>198</v>
       </c>
       <c r="D66" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E66" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F66" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G66" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="H66">
         <v>2</v>
@@ -2849,13 +2929,13 @@
         <v>200</v>
       </c>
       <c r="D67" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E67" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F67" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G67" t="s">
         <v>201</v>
@@ -2875,13 +2955,13 @@
         <v>203</v>
       </c>
       <c r="D68" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E68" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F68" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G68" t="s">
         <v>204</v>
@@ -2901,13 +2981,13 @@
         <v>206</v>
       </c>
       <c r="D69" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E69" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F69" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G69" t="s">
         <v>207</v>
@@ -2927,13 +3007,13 @@
         <v>209</v>
       </c>
       <c r="D70" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E70" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F70" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G70" t="s">
         <v>210</v>
@@ -2953,13 +3033,13 @@
         <v>212</v>
       </c>
       <c r="D71" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E71" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F71" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G71" t="s">
         <v>213</v>
@@ -2979,16 +3059,16 @@
         <v>215</v>
       </c>
       <c r="D72" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E72" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F72" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G72" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="H72">
         <v>5</v>
@@ -3005,13 +3085,13 @@
         <v>217</v>
       </c>
       <c r="D73" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E73" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F73" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G73" t="s">
         <v>218</v>
@@ -3031,13 +3111,13 @@
         <v>220</v>
       </c>
       <c r="D74" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E74" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F74" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G74" t="s">
         <v>221</v>
@@ -3057,13 +3137,13 @@
         <v>223</v>
       </c>
       <c r="D75" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E75" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F75" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="G75" t="s">
         <v>224</v>
@@ -3083,13 +3163,13 @@
         <v>226</v>
       </c>
       <c r="D76" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E76" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F76" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="G76" t="s">
         <v>207</v>
@@ -3109,13 +3189,13 @@
         <v>228</v>
       </c>
       <c r="D77" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E77" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F77" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="G77" t="s">
         <v>229</v>
@@ -3135,13 +3215,13 @@
         <v>231</v>
       </c>
       <c r="D78" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E78" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F78" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="G78" t="s">
         <v>232</v>
@@ -3161,13 +3241,13 @@
         <v>234</v>
       </c>
       <c r="D79" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E79" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F79" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="G79" t="s">
         <v>235</v>
@@ -3187,13 +3267,13 @@
         <v>237</v>
       </c>
       <c r="D80" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E80" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F80" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="G80" t="s">
         <v>238</v>
@@ -3213,13 +3293,13 @@
         <v>240</v>
       </c>
       <c r="D81" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E81" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F81" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="G81" t="s">
         <v>241</v>
@@ -3239,16 +3319,16 @@
         <v>243</v>
       </c>
       <c r="D82" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E82" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F82" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="G82" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="H82">
         <v>10</v>
@@ -3265,13 +3345,13 @@
         <v>245</v>
       </c>
       <c r="D83" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E83" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F83" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="G83" t="s">
         <v>246</v>
@@ -3291,13 +3371,13 @@
         <v>248</v>
       </c>
       <c r="D84" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E84" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F84" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="G84" t="s">
         <v>249</v>
@@ -3317,13 +3397,13 @@
         <v>251</v>
       </c>
       <c r="D85" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E85" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F85" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="G85" t="s">
         <v>193</v>
@@ -3343,13 +3423,13 @@
         <v>253</v>
       </c>
       <c r="D86" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E86" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F86" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="G86" t="s">
         <v>254</v>
@@ -3369,13 +3449,13 @@
         <v>256</v>
       </c>
       <c r="D87" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E87" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F87" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="G87" t="s">
         <v>257</v>
@@ -3395,13 +3475,13 @@
         <v>259</v>
       </c>
       <c r="D88" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E88" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F88" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="G88" t="s">
         <v>260</v>
@@ -3421,13 +3501,13 @@
         <v>262</v>
       </c>
       <c r="D89" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E89" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F89" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="G89" t="s">
         <v>263</v>
@@ -3447,10 +3527,10 @@
         <v>265</v>
       </c>
       <c r="D90" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E90" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F90" t="s">
         <v>266</v>
@@ -3473,10 +3553,10 @@
         <v>269</v>
       </c>
       <c r="D91" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E91" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F91" t="s">
         <v>270</v>
@@ -3499,10 +3579,10 @@
         <v>273</v>
       </c>
       <c r="D92" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E92" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F92" t="s">
         <v>266</v>
@@ -3525,10 +3605,10 @@
         <v>276</v>
       </c>
       <c r="D93" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E93" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F93" t="s">
         <v>270</v>
@@ -3551,10 +3631,10 @@
         <v>279</v>
       </c>
       <c r="D94" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E94" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F94" t="s">
         <v>270</v>
@@ -3577,10 +3657,10 @@
         <v>282</v>
       </c>
       <c r="D95" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E95" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F95" t="s">
         <v>266</v>
@@ -3603,10 +3683,10 @@
         <v>285</v>
       </c>
       <c r="D96" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E96" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F96" t="s">
         <v>266</v>
@@ -3629,10 +3709,10 @@
         <v>288</v>
       </c>
       <c r="D97" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E97" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F97" t="s">
         <v>270</v>
@@ -3655,10 +3735,10 @@
         <v>291</v>
       </c>
       <c r="D98" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E98" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F98" t="s">
         <v>266</v>
@@ -3681,16 +3761,16 @@
         <v>293</v>
       </c>
       <c r="D99" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E99" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F99" t="s">
         <v>270</v>
       </c>
       <c r="G99" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="H99">
         <v>18</v>
@@ -3707,10 +3787,10 @@
         <v>295</v>
       </c>
       <c r="D100" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E100" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F100" t="s">
         <v>270</v>
@@ -3733,10 +3813,10 @@
         <v>298</v>
       </c>
       <c r="D101" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E101" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F101" t="s">
         <v>266</v>
@@ -3759,10 +3839,10 @@
         <v>301</v>
       </c>
       <c r="D102" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E102" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F102" t="s">
         <v>270</v>
@@ -3785,10 +3865,10 @@
         <v>304</v>
       </c>
       <c r="D103" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E103" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F103" t="s">
         <v>266</v>
@@ -3801,7 +3881,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
Add conditions to starting card and add item cards
</commit_message>
<xml_diff>
--- a/scripts/cards.xlsx
+++ b/scripts/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\navarog\projects\expeditions\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF21F2C3-8B62-4264-A6D0-F41991DF9460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A4EFC6-9E77-4305-8390-E6AC8F05D463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="305">
   <si>
     <t>name</t>
   </si>
@@ -187,9 +187,6 @@
     <t>Synergy Halo</t>
   </si>
   <si>
-    <t>Whenever you gain at least 2 [Guile] during your turn, also gain [Power].</t>
-  </si>
-  <si>
     <t>Universal Vise</t>
   </si>
   <si>
@@ -229,9 +226,6 @@
     <t>Once per turn, if you rescue another card, either gain its core value or activate its ability.</t>
   </si>
   <si>
-    <t>Resque [ResqueCard]</t>
-  </si>
-  <si>
     <t>Chaos Grenade</t>
   </si>
   <si>
@@ -361,234 +355,156 @@
     <t>Fusion Link</t>
   </si>
   <si>
-    <t>Whenever you gain at least 2 [Power] during your turn, also gain [Guile].</t>
-  </si>
-  <si>
     <t>Mindstone</t>
   </si>
   <si>
     <t>meteorite</t>
   </si>
   <si>
-    <t>Place a worker on an active card to activate its ability. 2 [PurpleArrow] Gain [Power] per placed worker.</t>
-  </si>
-  <si>
     <t>Gain $1 per placed worker (max $3).</t>
   </si>
   <si>
     <t>Sunstone</t>
   </si>
   <si>
-    <t>Vanquish. 2 [PurpleArrow] Gain [Guile] per 3-value corruption.</t>
-  </si>
-  <si>
     <t>Gain $1 per 3-value corruption (max $3).</t>
   </si>
   <si>
     <t>Yellowstone</t>
   </si>
   <si>
-    <t>Gain 1 face-up yellow card to your hand. 2 [PurpleArrow] Gain [Power] per yellow card you control.</t>
-  </si>
-  <si>
     <t>Gain $1 per yellow card you control (max $3).</t>
   </si>
   <si>
     <t>Goldstone</t>
   </si>
   <si>
-    <t>Gather. 2 [PurpleArrow] Gain [Power] per adjacent location.</t>
-  </si>
-  <si>
     <t>Gain $1 per adjacent location.</t>
   </si>
   <si>
     <t>Leechstone</t>
   </si>
   <si>
-    <t>Refresh. 2 [PurpleArrow] Gain [Power] per player.</t>
-  </si>
-  <si>
     <t>Gain $1 per player.</t>
   </si>
   <si>
     <t>Cluestone</t>
   </si>
   <si>
-    <t>Solve. 2 [PurpleArrow] Gain [Power] per solved quest.</t>
-  </si>
-  <si>
     <t>Gain $1 per solved quest.</t>
   </si>
   <si>
     <t>Bravestone</t>
   </si>
   <si>
-    <t>Vanquish. 2 [PurpleArrow] Gain [Power] per 4-value corruption.</t>
-  </si>
-  <si>
     <t>Gain $1 per 4-value corruption (max $3).</t>
   </si>
   <si>
     <t>Charterstone</t>
   </si>
   <si>
-    <t>Move to any unoccupied face-up location. 2 [PurpleArrow] Gain [Guile] per adjacent face-up card.</t>
-  </si>
-  <si>
     <t>Gain $1 per adjacent face-up card.</t>
   </si>
   <si>
     <t>Greenstone</t>
   </si>
   <si>
-    <t>Gain 1 face-up green card to your hand. 2 [PurpleArrow] Gain [Guile] per green card you control.</t>
-  </si>
-  <si>
     <t>Gain $1 per green card you control (max $3).</t>
   </si>
   <si>
     <t>Mapstone</t>
   </si>
   <si>
-    <t>Gain a map from the general supply. 2 [PurpleArrow] Gain [Power] per map.</t>
-  </si>
-  <si>
     <t>Gain $1 per map (max $3).</t>
   </si>
   <si>
     <t>Redstone</t>
   </si>
   <si>
-    <t>Gain 1 face-up red card to your hand. 2 [PurpleArrow] Gain [Guile] per red card you control.</t>
-  </si>
-  <si>
     <t>Gain $1 per red card you control (max $3).</t>
   </si>
   <si>
     <t>Aidstone</t>
   </si>
   <si>
-    <t>Vanquish. 2 [PurpleArrow] Gain [Guile] per orange corruption.</t>
-  </si>
-  <si>
     <t>Gain $1 per orange corruption (max $3).</t>
   </si>
   <si>
     <t>Herostone</t>
   </si>
   <si>
-    <t>Discard a card to gain its core value. 2 [PurpleArrow] Rescue the previous card.</t>
-  </si>
-  <si>
     <t>Gain $1 per color among cards in hand.</t>
   </si>
   <si>
     <t>Queststone</t>
   </si>
   <si>
-    <t>Gain 1 face-up quest to your hand. 2 [PurpleArrow] Gain [Guile] per quest you control.</t>
-  </si>
-  <si>
     <t>Gain $1 per quest you control (max $3).</t>
   </si>
   <si>
     <t>Alanstone</t>
   </si>
   <si>
-    <t>Gain a worker. 2 [PurpleArrow] Gain [Guile] per available worker.</t>
-  </si>
-  <si>
     <t>Gain $1 per available worker (max $3).</t>
   </si>
   <si>
     <t>Brainstone</t>
   </si>
   <si>
-    <t>Gain 1 face-up item to your hand. 2 [PurpleArrow] Gain [Power] per item in your hand.</t>
-  </si>
-  <si>
     <t>Gain $1 per item you control (max $3).</t>
   </si>
   <si>
     <t>Gearstone</t>
   </si>
   <si>
-    <t>Upgrade. 2 [PurpleArrow] Gain [Power] per upgrade.</t>
-  </si>
-  <si>
     <t>Gain $1 per upgrade.</t>
   </si>
   <si>
     <t>Bluestone</t>
   </si>
   <si>
-    <t>Gain 1 face-up blue card to your hand. 2 [PurpleArrow] Gain [Power] per blue card you control.</t>
-  </si>
-  <si>
     <t>Gain $1 per blue card you control (max $3).</t>
   </si>
   <si>
     <t>Fuelstone</t>
   </si>
   <si>
-    <t>Vanquish. 2 [PurpleArrow] Gain [Power] per turquoise corruption.</t>
-  </si>
-  <si>
     <t>Gain $1 per turquoise corruption (max $3).</t>
   </si>
   <si>
     <t>Cipherstone</t>
   </si>
   <si>
-    <t>Discard a card to activate its ability. 2 [PurpleArrow] Gain the previous card’s core value.</t>
-  </si>
-  <si>
     <t>Gain $1 per active card (max $3).</t>
   </si>
   <si>
     <t>Purplestone</t>
   </si>
   <si>
-    <t>Gain 1 face-up purple card to your hand. 2 [PurpleArrow] Gain [Guile] per purple card you control.</t>
-  </si>
-  <si>
     <t>Gain $1 per purple card you control (max $3).</t>
   </si>
   <si>
     <t>Cullstone</t>
   </si>
   <si>
-    <t>Vanquish. 2 [PurpleArrow] Gain [Power] per 5-value corruption.</t>
-  </si>
-  <si>
     <t>Gain $1 per 5-value corruption (max $3).</t>
   </si>
   <si>
     <t>Aetherstone</t>
   </si>
   <si>
-    <t>Gain 1 face-up meteorite to your hand. 2 [PurpleArrow] Gain [Guile] per meteorite you control.</t>
-  </si>
-  <si>
     <t>Gain $1 per meteorite you control (max $3).</t>
   </si>
   <si>
     <t>Morphstone</t>
   </si>
   <si>
-    <t>Change a worker to purple; it becomes available. 2 [PurpleArrow] Gain [Power] per purple worker.</t>
-  </si>
-  <si>
     <t>Gain $1 per purple worker (max $3).</t>
   </si>
   <si>
     <t>Meldstone</t>
   </si>
   <si>
-    <t>Meld another meteorite. 2 [PurpleArrow] Gain [Guile] per melded meteorite.</t>
-  </si>
-  <si>
     <t>Gain $1 per melded meteorite.</t>
   </si>
   <si>
@@ -598,9 +514,6 @@
     <t>quest</t>
   </si>
   <si>
-    <t>If you have 0–2 cards in hand, gain 2 [Power]. Otherwise, gain [Guile].</t>
-  </si>
-  <si>
     <t>Play1Card</t>
   </si>
   <si>
@@ -640,9 +553,6 @@
     <t>Chart a Course North</t>
   </si>
   <si>
-    <t>Boast. If every opponent is south of you, gain 2 [Power].</t>
-  </si>
-  <si>
     <t>MapToken</t>
   </si>
   <si>
@@ -652,15 +562,9 @@
     <t>Gain [Guile] and rescue a card.</t>
   </si>
   <si>
-    <t>ResqueCard</t>
-  </si>
-  <si>
     <t>Drive off the Marauders</t>
   </si>
   <si>
-    <t>Discard a card to gain 2 [Power].</t>
-  </si>
-  <si>
     <t>ItemCard</t>
   </si>
   <si>
@@ -715,9 +619,6 @@
     <t>Unearth Some Strange Rocks</t>
   </si>
   <si>
-    <t>If you have no corruption, gain 2 [Guile]. Otherwise, gain 2 [Power].</t>
-  </si>
-  <si>
     <t>MeteoriteCard</t>
   </si>
   <si>
@@ -751,12 +652,6 @@
     <t>Placate Possessed Animals</t>
   </si>
   <si>
-    <t>Pay [Guile] to gain 2 [Power].</t>
-  </si>
-  <si>
-    <t>Resque a Trapped Mercenary</t>
-  </si>
-  <si>
     <t>Rescue another card; either gain its core value or activate its ability.</t>
   </si>
   <si>
@@ -808,9 +703,6 @@
     <t>Scout the Abandoned Base</t>
   </si>
   <si>
-    <t>Pay 2 [Guile] to gain the top corruption from an adjacent location if it’s a 3 or 4.</t>
-  </si>
-  <si>
     <t>GainAdjacentBenefit, Power</t>
   </si>
   <si>
@@ -823,9 +715,6 @@
     <t>Guile, Guile, Guile</t>
   </si>
   <si>
-    <t>PurpleArrow</t>
-  </si>
-  <si>
     <t>Recover a Stolen Map</t>
   </si>
   <si>
@@ -841,9 +730,6 @@
     <t>Activate the Ancient</t>
   </si>
   <si>
-    <t>Pay [Guile] to gain 3 [Power].</t>
-  </si>
-  <si>
     <t>Sweep, Power, Power</t>
   </si>
   <si>
@@ -907,18 +793,12 @@
     <t>Weaken the Leviathan</t>
   </si>
   <si>
-    <t>Gain 3 [Guile] if your mech is in the North, 2 [Guile] in Central, or [Guile] in the South.</t>
-  </si>
-  <si>
     <t>RescueCard, Coin</t>
   </si>
   <si>
     <t>Identify Members of a Lost Expedition</t>
   </si>
   <si>
-    <t>Gain [Guile] OR pay 2 [Guile] to gain $2.</t>
-  </si>
-  <si>
     <t>Play1Card, Coin</t>
   </si>
   <si>
@@ -938,6 +818,123 @@
   </si>
   <si>
     <t>MeeplePurple, Power</t>
+  </si>
+  <si>
+    <t>Place a worker on an active card to activate its ability. [Meld-2] Gain [Power] per placed worker.</t>
+  </si>
+  <si>
+    <t>Vanquish. [Meld-2] Gain [Guile] per 3-value corruption.</t>
+  </si>
+  <si>
+    <t>Gain 1 face-up yellow card to your hand. [Meld-2] Gain [Power] per yellow card you control.</t>
+  </si>
+  <si>
+    <t>Gather. [Meld-2] Gain [Power] per adjacent location.</t>
+  </si>
+  <si>
+    <t>Refresh. [Meld-2] Gain [Power] per player.</t>
+  </si>
+  <si>
+    <t>Solve. [Meld-2] Gain [Power] per solved quest.</t>
+  </si>
+  <si>
+    <t>Vanquish. [Meld-2] Gain [Power] per 4-value corruption.</t>
+  </si>
+  <si>
+    <t>Move to any unoccupied face-up location. [Meld-2] Gain [Guile] per adjacent face-up card.</t>
+  </si>
+  <si>
+    <t>Gain 1 face-up green card to your hand. [Meld-2] Gain [Guile] per green card you control.</t>
+  </si>
+  <si>
+    <t>Gain a map from the general supply. [Meld-2] Gain [Power] per map.</t>
+  </si>
+  <si>
+    <t>Gain 1 face-up red card to your hand. [Meld-2] Gain [Guile] per red card you control.</t>
+  </si>
+  <si>
+    <t>Vanquish. [Meld-2] Gain [Guile] per orange corruption.</t>
+  </si>
+  <si>
+    <t>Discard a card to gain its core value. [Meld-2] Rescue the previous card.</t>
+  </si>
+  <si>
+    <t>Gain 1 face-up quest to your hand. [Meld-2] Gain [Guile] per quest you control.</t>
+  </si>
+  <si>
+    <t>Gain a worker. [Meld-2] Gain [Guile] per available worker.</t>
+  </si>
+  <si>
+    <t>Gain 1 face-up item to your hand. [Meld-2] Gain [Power] per item in your hand.</t>
+  </si>
+  <si>
+    <t>Upgrade. [Meld-2] Gain [Power] per upgrade.</t>
+  </si>
+  <si>
+    <t>Gain 1 face-up blue card to your hand. [Meld-2] Gain [Power] per blue card you control.</t>
+  </si>
+  <si>
+    <t>Vanquish. [Meld-2] Gain [Power] per turquoise corruption.</t>
+  </si>
+  <si>
+    <t>Discard a card to activate its ability. [Meld-2] Gain the previous card’s core value.</t>
+  </si>
+  <si>
+    <t>Gain 1 face-up purple card to your hand. [Meld-2] Gain [Guile] per purple card you control.</t>
+  </si>
+  <si>
+    <t>Vanquish. [Meld-2] Gain [Power] per 5-value corruption.</t>
+  </si>
+  <si>
+    <t>Gain 1 face-up meteorite to your hand. [Meld-2] Gain [Guile] per meteorite you control.</t>
+  </si>
+  <si>
+    <t>Change a worker to purple; it becomes available. [Meld-2] Gain [Power] per purple worker.</t>
+  </si>
+  <si>
+    <t>Meld another meteorite. [Meld-2] Gain [Guile] per melded meteorite.</t>
+  </si>
+  <si>
+    <t>Whenever you gain at least 2x[Guile] during your turn, also gain [Power].</t>
+  </si>
+  <si>
+    <t>Pay 2x[Guile] to gain the top corruption from an adjacent location if it’s a 3 or 4.</t>
+  </si>
+  <si>
+    <t>Gain [Guile] OR pay 2x[Guile] to gain $2.</t>
+  </si>
+  <si>
+    <t>Gain 3x[Guile] if your mech is in the North, 2x[Guile] in Central, or [Guile] in the South.</t>
+  </si>
+  <si>
+    <t>Pay [Guile] to gain 3x[Power].</t>
+  </si>
+  <si>
+    <t>Whenever you gain at least 2x[Power] during your turn, also gain [Guile].</t>
+  </si>
+  <si>
+    <t>If you have 0–2 cards in hand, gain 2x[Power]. Otherwise, gain [Guile].</t>
+  </si>
+  <si>
+    <t>Boast. If every opponent is south of you, gain 2x[Power].</t>
+  </si>
+  <si>
+    <t>Discard a card to gain 2x[Power].</t>
+  </si>
+  <si>
+    <t>If you have no corruption, gain 2x[Guile]. Otherwise, gain 2x[Power].</t>
+  </si>
+  <si>
+    <t>Pay [Guile] to gain 2x[Power].</t>
+  </si>
+  <si>
+    <t>Rescue [RescueCard]</t>
+  </si>
+  <si>
+    <t>RescueCard</t>
+  </si>
+  <si>
+    <t>Rescue a Trapped Mercenary</t>
   </si>
 </sst>
 </file>
@@ -1002,6 +999,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1029,20 +1040,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1057,7 +1054,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F42030B-66C5-46F6-8CFB-CD633B482508}" name="Table1" displayName="Table1" ref="A1:K103" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F42030B-66C5-46F6-8CFB-CD633B482508}" name="Table1" displayName="Table1" ref="A1:K103" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:K103" xr:uid="{0F42030B-66C5-46F6-8CFB-CD633B482508}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C2006D74-3131-4AFC-AB17-9A5A423535C3}" name="name"/>
@@ -1363,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1747,7 +1744,7 @@
         <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>291</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
@@ -1764,13 +1761,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
         <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
@@ -1779,7 +1776,7 @@
         <v>21</v>
       </c>
       <c r="G17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J17">
         <v>3</v>
@@ -1787,13 +1784,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
         <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1802,18 +1799,18 @@
         <v>21</v>
       </c>
       <c r="G18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
         <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
         <v>31</v>
@@ -1822,7 +1819,7 @@
         <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J19">
         <v>4</v>
@@ -1830,13 +1827,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
         <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
         <v>31</v>
@@ -1845,7 +1842,7 @@
         <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J20">
         <v>2</v>
@@ -1853,13 +1850,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
         <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
         <v>31</v>
@@ -1868,7 +1865,7 @@
         <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>69</v>
+        <v>302</v>
       </c>
       <c r="J21">
         <v>3</v>
@@ -1876,13 +1873,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
         <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
         <v>31</v>
@@ -1891,7 +1888,7 @@
         <v>15</v>
       </c>
       <c r="G22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J22">
         <v>2</v>
@@ -1899,13 +1896,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
         <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
         <v>31</v>
@@ -1914,7 +1911,7 @@
         <v>15</v>
       </c>
       <c r="G23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J23">
         <v>4</v>
@@ -1922,13 +1919,13 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
@@ -1937,7 +1934,7 @@
         <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
+        <v>302</v>
       </c>
       <c r="J24">
         <v>2</v>
@@ -1945,13 +1942,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
         <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
@@ -1960,7 +1957,7 @@
         <v>21</v>
       </c>
       <c r="G25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J25">
         <v>2</v>
@@ -1968,13 +1965,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
         <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
         <v>14</v>
@@ -1983,7 +1980,7 @@
         <v>21</v>
       </c>
       <c r="G26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J26">
         <v>2</v>
@@ -1991,13 +1988,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
         <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D27" t="s">
         <v>14</v>
@@ -2006,7 +2003,7 @@
         <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J27">
         <v>4</v>
@@ -2014,13 +2011,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s">
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D28" t="s">
         <v>14</v>
@@ -2029,7 +2026,7 @@
         <v>21</v>
       </c>
       <c r="G28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J28">
         <v>2</v>
@@ -2037,13 +2034,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
         <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D29" t="s">
         <v>25</v>
@@ -2052,7 +2049,7 @@
         <v>21</v>
       </c>
       <c r="G29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J29">
         <v>4</v>
@@ -2060,13 +2057,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B30" t="s">
         <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s">
         <v>25</v>
@@ -2075,7 +2072,7 @@
         <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J30">
         <v>3</v>
@@ -2083,13 +2080,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
         <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D31" t="s">
         <v>25</v>
@@ -2098,7 +2095,7 @@
         <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J31">
         <v>4</v>
@@ -2106,13 +2103,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B32" t="s">
         <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D32" t="s">
         <v>25</v>
@@ -2121,7 +2118,7 @@
         <v>15</v>
       </c>
       <c r="G32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J32">
         <v>3</v>
@@ -2129,13 +2126,13 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B33" t="s">
         <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D33" t="s">
         <v>25</v>
@@ -2144,7 +2141,7 @@
         <v>21</v>
       </c>
       <c r="G33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J33">
         <v>3</v>
@@ -2152,22 +2149,22 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B34" t="s">
         <v>48</v>
       </c>
       <c r="C34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" t="s">
         <v>102</v>
-      </c>
-      <c r="D34" t="s">
-        <v>103</v>
-      </c>
-      <c r="E34" t="s">
-        <v>21</v>
-      </c>
-      <c r="G34" t="s">
-        <v>104</v>
       </c>
       <c r="J34">
         <v>3</v>
@@ -2175,22 +2172,22 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B35" t="s">
         <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
       </c>
       <c r="G35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J35">
         <v>2</v>
@@ -2198,22 +2195,22 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B36" t="s">
         <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E36" t="s">
         <v>21</v>
       </c>
       <c r="G36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J36">
         <v>2</v>
@@ -2221,22 +2218,22 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B37" t="s">
         <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E37" t="s">
         <v>21</v>
       </c>
       <c r="G37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J37">
         <v>3</v>
@@ -2244,22 +2241,22 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B38" t="s">
         <v>48</v>
       </c>
       <c r="C38" t="s">
-        <v>113</v>
+        <v>296</v>
       </c>
       <c r="D38" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
       </c>
       <c r="G38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J38">
         <v>4</v>
@@ -2267,13 +2264,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B39" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C39" t="s">
-        <v>116</v>
+        <v>266</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
@@ -2285,18 +2282,18 @@
         <v>21</v>
       </c>
       <c r="I39" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C40" t="s">
-        <v>119</v>
+        <v>267</v>
       </c>
       <c r="D40" t="s">
         <v>14</v>
@@ -2308,18 +2305,18 @@
         <v>15</v>
       </c>
       <c r="I40" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C41" t="s">
-        <v>122</v>
+        <v>268</v>
       </c>
       <c r="D41" t="s">
         <v>14</v>
@@ -2331,18 +2328,18 @@
         <v>21</v>
       </c>
       <c r="I41" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C42" t="s">
-        <v>125</v>
+        <v>269</v>
       </c>
       <c r="D42" t="s">
         <v>14</v>
@@ -2354,18 +2351,18 @@
         <v>21</v>
       </c>
       <c r="I42" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B43" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C43" t="s">
-        <v>128</v>
+        <v>270</v>
       </c>
       <c r="D43" t="s">
         <v>14</v>
@@ -2377,18 +2374,18 @@
         <v>21</v>
       </c>
       <c r="I43" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C44" t="s">
-        <v>131</v>
+        <v>271</v>
       </c>
       <c r="D44" t="s">
         <v>25</v>
@@ -2400,18 +2397,18 @@
         <v>21</v>
       </c>
       <c r="I44" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
-        <v>134</v>
+        <v>272</v>
       </c>
       <c r="D45" t="s">
         <v>25</v>
@@ -2423,18 +2420,18 @@
         <v>21</v>
       </c>
       <c r="I45" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B46" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C46" t="s">
-        <v>137</v>
+        <v>273</v>
       </c>
       <c r="D46" t="s">
         <v>25</v>
@@ -2446,18 +2443,18 @@
         <v>15</v>
       </c>
       <c r="I46" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C47" t="s">
-        <v>140</v>
+        <v>274</v>
       </c>
       <c r="D47" t="s">
         <v>25</v>
@@ -2469,18 +2466,18 @@
         <v>15</v>
       </c>
       <c r="I47" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B48" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C48" t="s">
-        <v>143</v>
+        <v>275</v>
       </c>
       <c r="D48" t="s">
         <v>25</v>
@@ -2492,18 +2489,18 @@
         <v>21</v>
       </c>
       <c r="I48" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C49" t="s">
-        <v>146</v>
+        <v>276</v>
       </c>
       <c r="D49" t="s">
         <v>31</v>
@@ -2515,18 +2512,18 @@
         <v>15</v>
       </c>
       <c r="I49" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="B50" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C50" t="s">
-        <v>149</v>
+        <v>277</v>
       </c>
       <c r="D50" t="s">
         <v>31</v>
@@ -2538,18 +2535,18 @@
         <v>15</v>
       </c>
       <c r="I50" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B51" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C51" t="s">
-        <v>152</v>
+        <v>278</v>
       </c>
       <c r="D51" t="s">
         <v>31</v>
@@ -2561,18 +2558,18 @@
         <v>15</v>
       </c>
       <c r="I51" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B52" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C52" t="s">
-        <v>155</v>
+        <v>279</v>
       </c>
       <c r="D52" t="s">
         <v>31</v>
@@ -2584,18 +2581,18 @@
         <v>15</v>
       </c>
       <c r="I52" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="B53" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C53" t="s">
-        <v>158</v>
+        <v>280</v>
       </c>
       <c r="D53" t="s">
         <v>31</v>
@@ -2607,18 +2604,18 @@
         <v>15</v>
       </c>
       <c r="I53" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C54" t="s">
-        <v>161</v>
+        <v>281</v>
       </c>
       <c r="D54" t="s">
         <v>20</v>
@@ -2630,18 +2627,18 @@
         <v>21</v>
       </c>
       <c r="I54" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="B55" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C55" t="s">
-        <v>164</v>
+        <v>282</v>
       </c>
       <c r="D55" t="s">
         <v>20</v>
@@ -2653,18 +2650,18 @@
         <v>21</v>
       </c>
       <c r="I55" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C56" t="s">
-        <v>167</v>
+        <v>283</v>
       </c>
       <c r="D56" t="s">
         <v>20</v>
@@ -2676,18 +2673,18 @@
         <v>21</v>
       </c>
       <c r="I56" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C57" t="s">
-        <v>170</v>
+        <v>284</v>
       </c>
       <c r="D57" t="s">
         <v>20</v>
@@ -2699,18 +2696,18 @@
         <v>21</v>
       </c>
       <c r="I57" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C58" t="s">
-        <v>173</v>
+        <v>285</v>
       </c>
       <c r="D58" t="s">
         <v>20</v>
@@ -2722,21 +2719,21 @@
         <v>21</v>
       </c>
       <c r="I58" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C59" t="s">
-        <v>176</v>
+        <v>286</v>
       </c>
       <c r="D59" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E59" t="s">
         <v>15</v>
@@ -2745,21 +2742,21 @@
         <v>15</v>
       </c>
       <c r="I59" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C60" t="s">
-        <v>179</v>
+        <v>287</v>
       </c>
       <c r="D60" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E60" t="s">
         <v>15</v>
@@ -2768,21 +2765,21 @@
         <v>15</v>
       </c>
       <c r="I60" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="B61" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C61" t="s">
-        <v>182</v>
+        <v>288</v>
       </c>
       <c r="D61" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E61" t="s">
         <v>21</v>
@@ -2791,21 +2788,21 @@
         <v>21</v>
       </c>
       <c r="I61" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="B62" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C62" t="s">
-        <v>185</v>
+        <v>289</v>
       </c>
       <c r="D62" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E62" t="s">
         <v>21</v>
@@ -2814,21 +2811,21 @@
         <v>21</v>
       </c>
       <c r="I62" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="B63" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C63" t="s">
-        <v>188</v>
+        <v>290</v>
       </c>
       <c r="D63" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E63" t="s">
         <v>15</v>
@@ -2837,18 +2834,18 @@
         <v>15</v>
       </c>
       <c r="I63" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="B64" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C64" t="s">
-        <v>192</v>
+        <v>297</v>
       </c>
       <c r="D64" t="s">
         <v>31</v>
@@ -2860,7 +2857,7 @@
         <v>15</v>
       </c>
       <c r="G64" t="s">
-        <v>193</v>
+        <v>164</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -2868,13 +2865,13 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>194</v>
+        <v>165</v>
       </c>
       <c r="B65" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C65" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
       <c r="D65" t="s">
         <v>20</v>
@@ -2886,7 +2883,7 @@
         <v>21</v>
       </c>
       <c r="G65" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -2894,13 +2891,13 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="B66" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C66" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="D66" t="s">
         <v>14</v>
@@ -2920,13 +2917,13 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="B67" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C67" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="D67" t="s">
         <v>20</v>
@@ -2938,7 +2935,7 @@
         <v>15</v>
       </c>
       <c r="G67" t="s">
-        <v>201</v>
+        <v>172</v>
       </c>
       <c r="H67">
         <v>2</v>
@@ -2946,16 +2943,16 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>202</v>
+        <v>173</v>
       </c>
       <c r="B68" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C68" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="D68" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E68" t="s">
         <v>21</v>
@@ -2964,7 +2961,7 @@
         <v>21</v>
       </c>
       <c r="G68" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="H68">
         <v>3</v>
@@ -2972,13 +2969,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
       <c r="B69" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C69" t="s">
-        <v>206</v>
+        <v>298</v>
       </c>
       <c r="D69" t="s">
         <v>25</v>
@@ -2990,7 +2987,7 @@
         <v>21</v>
       </c>
       <c r="G69" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="H69">
         <v>3</v>
@@ -2998,13 +2995,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="B70" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C70" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="D70" t="s">
         <v>14</v>
@@ -3016,7 +3013,7 @@
         <v>21</v>
       </c>
       <c r="G70" t="s">
-        <v>210</v>
+        <v>303</v>
       </c>
       <c r="H70">
         <v>4</v>
@@ -3024,13 +3021,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>211</v>
+        <v>180</v>
       </c>
       <c r="B71" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C71" t="s">
-        <v>212</v>
+        <v>299</v>
       </c>
       <c r="D71" t="s">
         <v>31</v>
@@ -3042,7 +3039,7 @@
         <v>15</v>
       </c>
       <c r="G71" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="H71">
         <v>4</v>
@@ -3050,13 +3047,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="B72" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C72" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
       <c r="D72" t="s">
         <v>20</v>
@@ -3076,16 +3073,16 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="B73" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C73" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="D73" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E73" t="s">
         <v>15</v>
@@ -3094,7 +3091,7 @@
         <v>15</v>
       </c>
       <c r="G73" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
       <c r="H73">
         <v>5</v>
@@ -3102,13 +3099,13 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
       <c r="B74" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C74" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="D74" t="s">
         <v>31</v>
@@ -3120,7 +3117,7 @@
         <v>15</v>
       </c>
       <c r="G74" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="H74">
         <v>6</v>
@@ -3128,13 +3125,13 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="B75" t="s">
+        <v>163</v>
+      </c>
+      <c r="C75" t="s">
         <v>191</v>
-      </c>
-      <c r="C75" t="s">
-        <v>223</v>
       </c>
       <c r="D75" t="s">
         <v>25</v>
@@ -3146,7 +3143,7 @@
         <v>15</v>
       </c>
       <c r="G75" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="H75">
         <v>6</v>
@@ -3154,13 +3151,13 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="B76" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C76" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="D76" t="s">
         <v>20</v>
@@ -3172,7 +3169,7 @@
         <v>22</v>
       </c>
       <c r="G76" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="H76">
         <v>7</v>
@@ -3180,13 +3177,13 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="B77" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C77" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="D77" t="s">
         <v>25</v>
@@ -3198,7 +3195,7 @@
         <v>40</v>
       </c>
       <c r="G77" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="H77">
         <v>7</v>
@@ -3206,16 +3203,16 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="B78" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C78" t="s">
-        <v>231</v>
+        <v>300</v>
       </c>
       <c r="D78" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E78" t="s">
         <v>15</v>
@@ -3224,7 +3221,7 @@
         <v>40</v>
       </c>
       <c r="G78" t="s">
-        <v>232</v>
+        <v>199</v>
       </c>
       <c r="H78">
         <v>8</v>
@@ -3232,16 +3229,16 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>233</v>
+        <v>200</v>
       </c>
       <c r="B79" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C79" t="s">
-        <v>234</v>
+        <v>201</v>
       </c>
       <c r="D79" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E79" t="s">
         <v>21</v>
@@ -3250,7 +3247,7 @@
         <v>22</v>
       </c>
       <c r="G79" t="s">
-        <v>235</v>
+        <v>202</v>
       </c>
       <c r="H79">
         <v>8</v>
@@ -3258,13 +3255,13 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>236</v>
+        <v>203</v>
       </c>
       <c r="B80" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C80" t="s">
-        <v>237</v>
+        <v>204</v>
       </c>
       <c r="D80" t="s">
         <v>14</v>
@@ -3276,7 +3273,7 @@
         <v>40</v>
       </c>
       <c r="G80" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="H80">
         <v>9</v>
@@ -3284,13 +3281,13 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>239</v>
+        <v>206</v>
       </c>
       <c r="B81" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C81" t="s">
-        <v>240</v>
+        <v>207</v>
       </c>
       <c r="D81" t="s">
         <v>14</v>
@@ -3302,7 +3299,7 @@
         <v>22</v>
       </c>
       <c r="G81" t="s">
-        <v>241</v>
+        <v>208</v>
       </c>
       <c r="H81">
         <v>9</v>
@@ -3310,13 +3307,13 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>242</v>
+        <v>209</v>
       </c>
       <c r="B82" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C82" t="s">
-        <v>243</v>
+        <v>301</v>
       </c>
       <c r="D82" t="s">
         <v>20</v>
@@ -3336,13 +3333,13 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>244</v>
+        <v>304</v>
       </c>
       <c r="B83" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C83" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="D83" t="s">
         <v>31</v>
@@ -3354,7 +3351,7 @@
         <v>40</v>
       </c>
       <c r="G83" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="H83">
         <v>10</v>
@@ -3362,13 +3359,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="B84" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C84" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="D84" t="s">
         <v>31</v>
@@ -3380,7 +3377,7 @@
         <v>40</v>
       </c>
       <c r="G84" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="H84">
         <v>11</v>
@@ -3388,13 +3385,13 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="B85" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C85" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
       <c r="D85" t="s">
         <v>25</v>
@@ -3406,7 +3403,7 @@
         <v>22</v>
       </c>
       <c r="G85" t="s">
-        <v>193</v>
+        <v>164</v>
       </c>
       <c r="H85">
         <v>11</v>
@@ -3414,13 +3411,13 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
       <c r="B86" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C86" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
       <c r="D86" t="s">
         <v>14</v>
@@ -3432,7 +3429,7 @@
         <v>40</v>
       </c>
       <c r="G86" t="s">
-        <v>254</v>
+        <v>219</v>
       </c>
       <c r="H86">
         <v>12</v>
@@ -3440,13 +3437,13 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="B87" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C87" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
       <c r="D87" t="s">
         <v>20</v>
@@ -3458,7 +3455,7 @@
         <v>22</v>
       </c>
       <c r="G87" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
       <c r="H87">
         <v>12</v>
@@ -3466,13 +3463,13 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>258</v>
+        <v>223</v>
       </c>
       <c r="B88" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C88" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="D88" t="s">
         <v>31</v>
@@ -3484,7 +3481,7 @@
         <v>40</v>
       </c>
       <c r="G88" t="s">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="H88">
         <v>13</v>
@@ -3492,13 +3489,13 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="B89" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C89" t="s">
-        <v>262</v>
+        <v>292</v>
       </c>
       <c r="D89" t="s">
         <v>31</v>
@@ -3510,7 +3507,7 @@
         <v>22</v>
       </c>
       <c r="G89" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="H89">
         <v>13</v>
@@ -3518,13 +3515,13 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="B90" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C90" t="s">
-        <v>265</v>
+        <v>229</v>
       </c>
       <c r="D90" t="s">
         <v>14</v>
@@ -3533,10 +3530,10 @@
         <v>21</v>
       </c>
       <c r="F90" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="G90" t="s">
-        <v>267</v>
+        <v>109</v>
       </c>
       <c r="H90">
         <v>14</v>
@@ -3544,13 +3541,13 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>268</v>
+        <v>231</v>
       </c>
       <c r="B91" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C91" t="s">
-        <v>269</v>
+        <v>232</v>
       </c>
       <c r="D91" t="s">
         <v>25</v>
@@ -3559,10 +3556,10 @@
         <v>21</v>
       </c>
       <c r="F91" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
       <c r="G91" t="s">
-        <v>271</v>
+        <v>234</v>
       </c>
       <c r="H91">
         <v>14</v>
@@ -3570,13 +3567,13 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>272</v>
+        <v>235</v>
       </c>
       <c r="B92" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C92" t="s">
-        <v>273</v>
+        <v>295</v>
       </c>
       <c r="D92" t="s">
         <v>20</v>
@@ -3585,10 +3582,10 @@
         <v>21</v>
       </c>
       <c r="F92" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="G92" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="H92">
         <v>15</v>
@@ -3596,25 +3593,25 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="B93" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C93" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="D93" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E93" t="s">
         <v>21</v>
       </c>
       <c r="F93" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
       <c r="G93" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
       <c r="H93">
         <v>15</v>
@@ -3622,13 +3619,13 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="B94" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C94" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
       <c r="D94" t="s">
         <v>31</v>
@@ -3637,10 +3634,10 @@
         <v>15</v>
       </c>
       <c r="F94" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
       <c r="G94" t="s">
-        <v>280</v>
+        <v>242</v>
       </c>
       <c r="H94">
         <v>16</v>
@@ -3648,25 +3645,25 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>281</v>
+        <v>243</v>
       </c>
       <c r="B95" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C95" t="s">
-        <v>282</v>
+        <v>244</v>
       </c>
       <c r="D95" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E95" t="s">
         <v>15</v>
       </c>
       <c r="F95" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="G95" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
       <c r="H95">
         <v>16</v>
@@ -3674,13 +3671,13 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>284</v>
+        <v>246</v>
       </c>
       <c r="B96" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C96" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="D96" t="s">
         <v>14</v>
@@ -3689,10 +3686,10 @@
         <v>21</v>
       </c>
       <c r="F96" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="G96" t="s">
-        <v>286</v>
+        <v>248</v>
       </c>
       <c r="H96">
         <v>17</v>
@@ -3700,25 +3697,25 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>287</v>
+        <v>249</v>
       </c>
       <c r="B97" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C97" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="D97" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E97" t="s">
         <v>21</v>
       </c>
       <c r="F97" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
       <c r="G97" t="s">
-        <v>289</v>
+        <v>251</v>
       </c>
       <c r="H97">
         <v>17</v>
@@ -3726,13 +3723,13 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>290</v>
+        <v>252</v>
       </c>
       <c r="B98" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C98" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="D98" t="s">
         <v>25</v>
@@ -3741,10 +3738,10 @@
         <v>21</v>
       </c>
       <c r="F98" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="G98" t="s">
-        <v>235</v>
+        <v>202</v>
       </c>
       <c r="H98">
         <v>18</v>
@@ -3752,13 +3749,13 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="B99" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C99" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="D99" t="s">
         <v>20</v>
@@ -3767,10 +3764,10 @@
         <v>15</v>
       </c>
       <c r="F99" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
       <c r="G99" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H99">
         <v>18</v>
@@ -3778,13 +3775,13 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>256</v>
+      </c>
+      <c r="B100" t="s">
+        <v>163</v>
+      </c>
+      <c r="C100" t="s">
         <v>294</v>
-      </c>
-      <c r="B100" t="s">
-        <v>191</v>
-      </c>
-      <c r="C100" t="s">
-        <v>295</v>
       </c>
       <c r="D100" t="s">
         <v>25</v>
@@ -3793,10 +3790,10 @@
         <v>15</v>
       </c>
       <c r="F100" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
       <c r="G100" t="s">
-        <v>296</v>
+        <v>257</v>
       </c>
       <c r="H100">
         <v>19</v>
@@ -3804,13 +3801,13 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>297</v>
+        <v>258</v>
       </c>
       <c r="B101" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C101" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D101" t="s">
         <v>14</v>
@@ -3819,10 +3816,10 @@
         <v>21</v>
       </c>
       <c r="F101" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="G101" t="s">
-        <v>299</v>
+        <v>259</v>
       </c>
       <c r="H101">
         <v>19</v>
@@ -3830,13 +3827,13 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="B102" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C102" t="s">
-        <v>301</v>
+        <v>261</v>
       </c>
       <c r="D102" t="s">
         <v>20</v>
@@ -3845,10 +3842,10 @@
         <v>21</v>
       </c>
       <c r="F102" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
       <c r="G102" t="s">
-        <v>302</v>
+        <v>262</v>
       </c>
       <c r="H102">
         <v>20</v>
@@ -3856,25 +3853,25 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>303</v>
+        <v>263</v>
       </c>
       <c r="B103" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C103" t="s">
-        <v>304</v>
+        <v>264</v>
       </c>
       <c r="D103" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E103" t="s">
         <v>15</v>
       </c>
       <c r="F103" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="G103" t="s">
-        <v>305</v>
+        <v>265</v>
       </c>
       <c r="H103">
         <v>20</v>

</xml_diff>

<commit_message>
Add meteorite and quest card layouts
</commit_message>
<xml_diff>
--- a/scripts/cards.xlsx
+++ b/scripts/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\navarog\projects\expeditions\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A4EFC6-9E77-4305-8390-E6AC8F05D463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E865557-84C4-4214-BB8A-E6D70438A51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -523,9 +523,6 @@
     <t>Gain [Guile] OR Upgrade.</t>
   </si>
   <si>
-    <t>MeepleBlue</t>
-  </si>
-  <si>
     <t>Interrogate Meteorite Eyewitnesses</t>
   </si>
   <si>
@@ -655,18 +652,12 @@
     <t>Rescue another card; either gain its core value or activate its ability.</t>
   </si>
   <si>
-    <t>MeepleRed</t>
-  </si>
-  <si>
     <t>Clear a Path into the Town</t>
   </si>
   <si>
     <t>Gain the core value of all adjacent face–up cards, then sweep only those cards.</t>
   </si>
   <si>
-    <t>ActivateAdjancentBenefit, Guile</t>
-  </si>
-  <si>
     <t>Search the Mining Town for Fuel and Survivors</t>
   </si>
   <si>
@@ -679,9 +670,6 @@
     <t>Gain [Power] OR pay 5x[Power] to gain $3.</t>
   </si>
   <si>
-    <t>MeepleGreen, Guile</t>
-  </si>
-  <si>
     <t>Cure a Whale of Parasites</t>
   </si>
   <si>
@@ -748,9 +736,6 @@
     <t>Rescue another card. If it had a worker on it, gain [Guile][Power].</t>
   </si>
   <si>
-    <t>MeepleYellow, Coin</t>
-  </si>
-  <si>
     <t>Study Meteorites on the Village Outskirts</t>
   </si>
   <si>
@@ -775,9 +760,6 @@
     <t>Transfer the top corruption from each adjacent location to your location.</t>
   </si>
   <si>
-    <t>ActivateAdjancentBenefit, Coin</t>
-  </si>
-  <si>
     <t>Find a Secret Passage</t>
   </si>
   <si>
@@ -817,9 +799,6 @@
     <t>Activate the ability of any face–up purple card, then gain that card.</t>
   </si>
   <si>
-    <t>MeeplePurple, Power</t>
-  </si>
-  <si>
     <t>Place a worker on an active card to activate its ability. [Meld-2] Gain [Power] per placed worker.</t>
   </si>
   <si>
@@ -935,6 +914,27 @@
   </si>
   <si>
     <t>Rescue a Trapped Mercenary</t>
+  </si>
+  <si>
+    <t>WorkerBlue</t>
+  </si>
+  <si>
+    <t>WorkerRed</t>
+  </si>
+  <si>
+    <t>WorkerGreen, Guile</t>
+  </si>
+  <si>
+    <t>WorkerYellow, Coin</t>
+  </si>
+  <si>
+    <t>WorkerPurple, Power</t>
+  </si>
+  <si>
+    <t>ActivateAdjacentBenefit, Guile</t>
+  </si>
+  <si>
+    <t>ActivateAdjacentBenefit, Coin</t>
   </si>
 </sst>
 </file>
@@ -1360,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1744,7 +1744,7 @@
         <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
@@ -1801,6 +1801,9 @@
       <c r="G18" t="s">
         <v>60</v>
       </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1865,7 +1868,7 @@
         <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="J21">
         <v>3</v>
@@ -1934,7 +1937,7 @@
         <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="J24">
         <v>2</v>
@@ -2247,7 +2250,7 @@
         <v>48</v>
       </c>
       <c r="C38" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D38" t="s">
         <v>101</v>
@@ -2270,7 +2273,7 @@
         <v>112</v>
       </c>
       <c r="C39" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
@@ -2293,7 +2296,7 @@
         <v>112</v>
       </c>
       <c r="C40" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="D40" t="s">
         <v>14</v>
@@ -2316,7 +2319,7 @@
         <v>112</v>
       </c>
       <c r="C41" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="D41" t="s">
         <v>14</v>
@@ -2339,7 +2342,7 @@
         <v>112</v>
       </c>
       <c r="C42" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D42" t="s">
         <v>14</v>
@@ -2362,7 +2365,7 @@
         <v>112</v>
       </c>
       <c r="C43" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="D43" t="s">
         <v>14</v>
@@ -2385,7 +2388,7 @@
         <v>112</v>
       </c>
       <c r="C44" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D44" t="s">
         <v>25</v>
@@ -2408,7 +2411,7 @@
         <v>112</v>
       </c>
       <c r="C45" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D45" t="s">
         <v>25</v>
@@ -2431,7 +2434,7 @@
         <v>112</v>
       </c>
       <c r="C46" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D46" t="s">
         <v>25</v>
@@ -2454,7 +2457,7 @@
         <v>112</v>
       </c>
       <c r="C47" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="D47" t="s">
         <v>25</v>
@@ -2477,7 +2480,7 @@
         <v>112</v>
       </c>
       <c r="C48" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D48" t="s">
         <v>25</v>
@@ -2500,7 +2503,7 @@
         <v>112</v>
       </c>
       <c r="C49" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="D49" t="s">
         <v>31</v>
@@ -2523,7 +2526,7 @@
         <v>112</v>
       </c>
       <c r="C50" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="D50" t="s">
         <v>31</v>
@@ -2546,7 +2549,7 @@
         <v>112</v>
       </c>
       <c r="C51" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D51" t="s">
         <v>31</v>
@@ -2569,7 +2572,7 @@
         <v>112</v>
       </c>
       <c r="C52" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="D52" t="s">
         <v>31</v>
@@ -2592,7 +2595,7 @@
         <v>112</v>
       </c>
       <c r="C53" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D53" t="s">
         <v>31</v>
@@ -2615,7 +2618,7 @@
         <v>112</v>
       </c>
       <c r="C54" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="D54" t="s">
         <v>20</v>
@@ -2638,7 +2641,7 @@
         <v>112</v>
       </c>
       <c r="C55" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D55" t="s">
         <v>20</v>
@@ -2661,7 +2664,7 @@
         <v>112</v>
       </c>
       <c r="C56" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D56" t="s">
         <v>20</v>
@@ -2684,7 +2687,7 @@
         <v>112</v>
       </c>
       <c r="C57" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D57" t="s">
         <v>20</v>
@@ -2707,7 +2710,7 @@
         <v>112</v>
       </c>
       <c r="C58" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="D58" t="s">
         <v>20</v>
@@ -2730,7 +2733,7 @@
         <v>112</v>
       </c>
       <c r="C59" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="D59" t="s">
         <v>101</v>
@@ -2753,7 +2756,7 @@
         <v>112</v>
       </c>
       <c r="C60" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="D60" t="s">
         <v>101</v>
@@ -2776,7 +2779,7 @@
         <v>112</v>
       </c>
       <c r="C61" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="D61" t="s">
         <v>101</v>
@@ -2799,7 +2802,7 @@
         <v>112</v>
       </c>
       <c r="C62" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="D62" t="s">
         <v>101</v>
@@ -2822,7 +2825,7 @@
         <v>112</v>
       </c>
       <c r="C63" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D63" t="s">
         <v>101</v>
@@ -2845,7 +2848,7 @@
         <v>163</v>
       </c>
       <c r="C64" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D64" t="s">
         <v>31</v>
@@ -2883,7 +2886,7 @@
         <v>21</v>
       </c>
       <c r="G65" t="s">
-        <v>167</v>
+        <v>298</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -2891,13 +2894,13 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>167</v>
+      </c>
+      <c r="B66" t="s">
+        <v>163</v>
+      </c>
+      <c r="C66" t="s">
         <v>168</v>
-      </c>
-      <c r="B66" t="s">
-        <v>163</v>
-      </c>
-      <c r="C66" t="s">
-        <v>169</v>
       </c>
       <c r="D66" t="s">
         <v>14</v>
@@ -2917,13 +2920,13 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>169</v>
+      </c>
+      <c r="B67" t="s">
+        <v>163</v>
+      </c>
+      <c r="C67" t="s">
         <v>170</v>
-      </c>
-      <c r="B67" t="s">
-        <v>163</v>
-      </c>
-      <c r="C67" t="s">
-        <v>171</v>
       </c>
       <c r="D67" t="s">
         <v>20</v>
@@ -2935,7 +2938,7 @@
         <v>15</v>
       </c>
       <c r="G67" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H67">
         <v>2</v>
@@ -2943,13 +2946,13 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>172</v>
+      </c>
+      <c r="B68" t="s">
+        <v>163</v>
+      </c>
+      <c r="C68" t="s">
         <v>173</v>
-      </c>
-      <c r="B68" t="s">
-        <v>163</v>
-      </c>
-      <c r="C68" t="s">
-        <v>174</v>
       </c>
       <c r="D68" t="s">
         <v>101</v>
@@ -2961,7 +2964,7 @@
         <v>21</v>
       </c>
       <c r="G68" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H68">
         <v>3</v>
@@ -2969,13 +2972,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B69" t="s">
         <v>163</v>
       </c>
       <c r="C69" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="D69" t="s">
         <v>25</v>
@@ -2987,7 +2990,7 @@
         <v>21</v>
       </c>
       <c r="G69" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H69">
         <v>3</v>
@@ -2995,13 +2998,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>177</v>
+      </c>
+      <c r="B70" t="s">
+        <v>163</v>
+      </c>
+      <c r="C70" t="s">
         <v>178</v>
-      </c>
-      <c r="B70" t="s">
-        <v>163</v>
-      </c>
-      <c r="C70" t="s">
-        <v>179</v>
       </c>
       <c r="D70" t="s">
         <v>14</v>
@@ -3013,7 +3016,7 @@
         <v>21</v>
       </c>
       <c r="G70" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="H70">
         <v>4</v>
@@ -3021,13 +3024,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B71" t="s">
         <v>163</v>
       </c>
       <c r="C71" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D71" t="s">
         <v>31</v>
@@ -3039,7 +3042,7 @@
         <v>15</v>
       </c>
       <c r="G71" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H71">
         <v>4</v>
@@ -3047,13 +3050,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B72" t="s">
+        <v>163</v>
+      </c>
+      <c r="C72" t="s">
         <v>182</v>
-      </c>
-      <c r="B72" t="s">
-        <v>163</v>
-      </c>
-      <c r="C72" t="s">
-        <v>183</v>
       </c>
       <c r="D72" t="s">
         <v>20</v>
@@ -3073,13 +3076,13 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>183</v>
+      </c>
+      <c r="B73" t="s">
+        <v>163</v>
+      </c>
+      <c r="C73" t="s">
         <v>184</v>
-      </c>
-      <c r="B73" t="s">
-        <v>163</v>
-      </c>
-      <c r="C73" t="s">
-        <v>185</v>
       </c>
       <c r="D73" t="s">
         <v>101</v>
@@ -3091,7 +3094,7 @@
         <v>15</v>
       </c>
       <c r="G73" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H73">
         <v>5</v>
@@ -3099,13 +3102,13 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>186</v>
+      </c>
+      <c r="B74" t="s">
+        <v>163</v>
+      </c>
+      <c r="C74" t="s">
         <v>187</v>
-      </c>
-      <c r="B74" t="s">
-        <v>163</v>
-      </c>
-      <c r="C74" t="s">
-        <v>188</v>
       </c>
       <c r="D74" t="s">
         <v>31</v>
@@ -3117,7 +3120,7 @@
         <v>15</v>
       </c>
       <c r="G74" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H74">
         <v>6</v>
@@ -3125,13 +3128,13 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>189</v>
+      </c>
+      <c r="B75" t="s">
+        <v>163</v>
+      </c>
+      <c r="C75" t="s">
         <v>190</v>
-      </c>
-      <c r="B75" t="s">
-        <v>163</v>
-      </c>
-      <c r="C75" t="s">
-        <v>191</v>
       </c>
       <c r="D75" t="s">
         <v>25</v>
@@ -3143,7 +3146,7 @@
         <v>15</v>
       </c>
       <c r="G75" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H75">
         <v>6</v>
@@ -3151,13 +3154,13 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>192</v>
+      </c>
+      <c r="B76" t="s">
+        <v>163</v>
+      </c>
+      <c r="C76" t="s">
         <v>193</v>
-      </c>
-      <c r="B76" t="s">
-        <v>163</v>
-      </c>
-      <c r="C76" t="s">
-        <v>194</v>
       </c>
       <c r="D76" t="s">
         <v>20</v>
@@ -3169,7 +3172,7 @@
         <v>22</v>
       </c>
       <c r="G76" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H76">
         <v>7</v>
@@ -3177,13 +3180,13 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>194</v>
+      </c>
+      <c r="B77" t="s">
+        <v>163</v>
+      </c>
+      <c r="C77" t="s">
         <v>195</v>
-      </c>
-      <c r="B77" t="s">
-        <v>163</v>
-      </c>
-      <c r="C77" t="s">
-        <v>196</v>
       </c>
       <c r="D77" t="s">
         <v>25</v>
@@ -3195,7 +3198,7 @@
         <v>40</v>
       </c>
       <c r="G77" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H77">
         <v>7</v>
@@ -3203,13 +3206,13 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B78" t="s">
         <v>163</v>
       </c>
       <c r="C78" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="D78" t="s">
         <v>101</v>
@@ -3221,7 +3224,7 @@
         <v>40</v>
       </c>
       <c r="G78" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H78">
         <v>8</v>
@@ -3229,13 +3232,13 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>199</v>
+      </c>
+      <c r="B79" t="s">
+        <v>163</v>
+      </c>
+      <c r="C79" t="s">
         <v>200</v>
-      </c>
-      <c r="B79" t="s">
-        <v>163</v>
-      </c>
-      <c r="C79" t="s">
-        <v>201</v>
       </c>
       <c r="D79" t="s">
         <v>101</v>
@@ -3247,7 +3250,7 @@
         <v>22</v>
       </c>
       <c r="G79" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H79">
         <v>8</v>
@@ -3255,13 +3258,13 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>202</v>
+      </c>
+      <c r="B80" t="s">
+        <v>163</v>
+      </c>
+      <c r="C80" t="s">
         <v>203</v>
-      </c>
-      <c r="B80" t="s">
-        <v>163</v>
-      </c>
-      <c r="C80" t="s">
-        <v>204</v>
       </c>
       <c r="D80" t="s">
         <v>14</v>
@@ -3273,7 +3276,7 @@
         <v>40</v>
       </c>
       <c r="G80" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H80">
         <v>9</v>
@@ -3281,13 +3284,13 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>205</v>
+      </c>
+      <c r="B81" t="s">
+        <v>163</v>
+      </c>
+      <c r="C81" t="s">
         <v>206</v>
-      </c>
-      <c r="B81" t="s">
-        <v>163</v>
-      </c>
-      <c r="C81" t="s">
-        <v>207</v>
       </c>
       <c r="D81" t="s">
         <v>14</v>
@@ -3299,7 +3302,7 @@
         <v>22</v>
       </c>
       <c r="G81" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H81">
         <v>9</v>
@@ -3307,13 +3310,13 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B82" t="s">
         <v>163</v>
       </c>
       <c r="C82" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D82" t="s">
         <v>20</v>
@@ -3333,13 +3336,13 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="B83" t="s">
         <v>163</v>
       </c>
       <c r="C83" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D83" t="s">
         <v>31</v>
@@ -3351,7 +3354,7 @@
         <v>40</v>
       </c>
       <c r="G83" t="s">
-        <v>211</v>
+        <v>299</v>
       </c>
       <c r="H83">
         <v>10</v>
@@ -3359,13 +3362,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B84" t="s">
         <v>163</v>
       </c>
       <c r="C84" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D84" t="s">
         <v>31</v>
@@ -3377,7 +3380,7 @@
         <v>40</v>
       </c>
       <c r="G84" t="s">
-        <v>214</v>
+        <v>303</v>
       </c>
       <c r="H84">
         <v>11</v>
@@ -3385,13 +3388,13 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B85" t="s">
         <v>163</v>
       </c>
       <c r="C85" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D85" t="s">
         <v>25</v>
@@ -3411,13 +3414,13 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B86" t="s">
         <v>163</v>
       </c>
       <c r="C86" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D86" t="s">
         <v>14</v>
@@ -3429,7 +3432,7 @@
         <v>40</v>
       </c>
       <c r="G86" t="s">
-        <v>219</v>
+        <v>300</v>
       </c>
       <c r="H86">
         <v>12</v>
@@ -3437,13 +3440,13 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B87" t="s">
         <v>163</v>
       </c>
       <c r="C87" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D87" t="s">
         <v>20</v>
@@ -3455,7 +3458,7 @@
         <v>22</v>
       </c>
       <c r="G87" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="H87">
         <v>12</v>
@@ -3463,13 +3466,13 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B88" t="s">
         <v>163</v>
       </c>
       <c r="C88" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D88" t="s">
         <v>31</v>
@@ -3481,7 +3484,7 @@
         <v>40</v>
       </c>
       <c r="G88" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H88">
         <v>13</v>
@@ -3489,13 +3492,13 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B89" t="s">
         <v>163</v>
       </c>
       <c r="C89" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="D89" t="s">
         <v>31</v>
@@ -3507,7 +3510,7 @@
         <v>22</v>
       </c>
       <c r="G89" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="H89">
         <v>13</v>
@@ -3515,13 +3518,13 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B90" t="s">
         <v>163</v>
       </c>
       <c r="C90" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D90" t="s">
         <v>14</v>
@@ -3530,7 +3533,7 @@
         <v>21</v>
       </c>
       <c r="F90" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G90" t="s">
         <v>109</v>
@@ -3541,13 +3544,13 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B91" t="s">
         <v>163</v>
       </c>
       <c r="C91" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D91" t="s">
         <v>25</v>
@@ -3556,10 +3559,10 @@
         <v>21</v>
       </c>
       <c r="F91" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G91" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H91">
         <v>14</v>
@@ -3567,13 +3570,13 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B92" t="s">
         <v>163</v>
       </c>
       <c r="C92" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D92" t="s">
         <v>20</v>
@@ -3582,10 +3585,10 @@
         <v>21</v>
       </c>
       <c r="F92" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G92" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H92">
         <v>15</v>
@@ -3593,13 +3596,13 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B93" t="s">
         <v>163</v>
       </c>
       <c r="C93" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D93" t="s">
         <v>101</v>
@@ -3608,10 +3611,10 @@
         <v>21</v>
       </c>
       <c r="F93" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G93" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="H93">
         <v>15</v>
@@ -3619,13 +3622,13 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B94" t="s">
         <v>163</v>
       </c>
       <c r="C94" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D94" t="s">
         <v>31</v>
@@ -3634,10 +3637,10 @@
         <v>15</v>
       </c>
       <c r="F94" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G94" t="s">
-        <v>242</v>
+        <v>301</v>
       </c>
       <c r="H94">
         <v>16</v>
@@ -3645,13 +3648,13 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B95" t="s">
         <v>163</v>
       </c>
       <c r="C95" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D95" t="s">
         <v>101</v>
@@ -3660,10 +3663,10 @@
         <v>15</v>
       </c>
       <c r="F95" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G95" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H95">
         <v>16</v>
@@ -3671,13 +3674,13 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B96" t="s">
         <v>163</v>
       </c>
       <c r="C96" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D96" t="s">
         <v>14</v>
@@ -3686,10 +3689,10 @@
         <v>21</v>
       </c>
       <c r="F96" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G96" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H96">
         <v>17</v>
@@ -3697,13 +3700,13 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B97" t="s">
         <v>163</v>
       </c>
       <c r="C97" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D97" t="s">
         <v>101</v>
@@ -3712,10 +3715,10 @@
         <v>21</v>
       </c>
       <c r="F97" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G97" t="s">
-        <v>251</v>
+        <v>304</v>
       </c>
       <c r="H97">
         <v>17</v>
@@ -3723,13 +3726,13 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B98" t="s">
         <v>163</v>
       </c>
       <c r="C98" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D98" t="s">
         <v>25</v>
@@ -3738,10 +3741,10 @@
         <v>21</v>
       </c>
       <c r="F98" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G98" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H98">
         <v>18</v>
@@ -3749,13 +3752,13 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B99" t="s">
         <v>163</v>
       </c>
       <c r="C99" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="D99" t="s">
         <v>20</v>
@@ -3764,7 +3767,7 @@
         <v>15</v>
       </c>
       <c r="F99" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G99" t="s">
         <v>57</v>
@@ -3775,13 +3778,13 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B100" t="s">
         <v>163</v>
       </c>
       <c r="C100" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="D100" t="s">
         <v>25</v>
@@ -3790,10 +3793,10 @@
         <v>15</v>
       </c>
       <c r="F100" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G100" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="H100">
         <v>19</v>
@@ -3801,13 +3804,13 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B101" t="s">
         <v>163</v>
       </c>
       <c r="C101" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="D101" t="s">
         <v>14</v>
@@ -3816,10 +3819,10 @@
         <v>21</v>
       </c>
       <c r="F101" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G101" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="H101">
         <v>19</v>
@@ -3827,13 +3830,13 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B102" t="s">
         <v>163</v>
       </c>
       <c r="C102" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D102" t="s">
         <v>20</v>
@@ -3842,10 +3845,10 @@
         <v>21</v>
       </c>
       <c r="F102" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G102" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="H102">
         <v>20</v>
@@ -3853,13 +3856,13 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B103" t="s">
         <v>163</v>
       </c>
       <c r="C103" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D103" t="s">
         <v>101</v>
@@ -3868,10 +3871,10 @@
         <v>15</v>
       </c>
       <c r="F103" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G103" t="s">
-        <v>265</v>
+        <v>302</v>
       </c>
       <c r="H103">
         <v>20</v>

</xml_diff>

<commit_message>
Add card IDs and index them
</commit_message>
<xml_diff>
--- a/scripts/cards.xlsx
+++ b/scripts/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\navarog\projects\expeditions\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E865557-84C4-4214-BB8A-E6D70438A51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8508A72-C689-4455-BC01-8D3194D7FEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="306">
   <si>
     <t>name</t>
   </si>
@@ -935,6 +935,9 @@
   </si>
   <si>
     <t>ActivateAdjacentBenefit, Coin</t>
+  </si>
+  <si>
+    <t>number</t>
   </si>
 </sst>
 </file>
@@ -1054,9 +1057,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F42030B-66C5-46F6-8CFB-CD633B482508}" name="Table1" displayName="Table1" ref="A1:K103" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:K103" xr:uid="{0F42030B-66C5-46F6-8CFB-CD633B482508}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F42030B-66C5-46F6-8CFB-CD633B482508}" name="Table1" displayName="Table1" ref="A1:L103" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:L103" xr:uid="{0F42030B-66C5-46F6-8CFB-CD633B482508}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{C2006D74-3131-4AFC-AB17-9A5A423535C3}" name="name"/>
     <tableColumn id="2" xr3:uid="{3C4235A7-DBEF-42F6-B2B8-B558B520A439}" name="type"/>
     <tableColumn id="3" xr3:uid="{9445079D-106C-44A3-BE10-AD4E28465146}" name="ability"/>
@@ -1068,6 +1071,7 @@
     <tableColumn id="9" xr3:uid="{0C1DFD4D-6D58-4BBF-9103-96680EC6E963}" name="meld"/>
     <tableColumn id="10" xr3:uid="{8BEE43DE-239D-482B-81BD-AA9B82DCD4C1}" name="coins"/>
     <tableColumn id="11" xr3:uid="{551EE5F0-3D63-4829-8E14-8064AD20AE34}" name="team"/>
+    <tableColumn id="12" xr3:uid="{C1F323AB-632E-4110-88B0-57C52F4B4481}" name="number"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1358,28 +1362,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K103"/>
+  <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" topLeftCell="D51" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14:L103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="141.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="141.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1413,8 +1417,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1437,7 +1444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1460,7 +1467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1483,7 +1490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1506,7 +1513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1529,7 +1536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1552,7 +1559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1575,7 +1582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1598,7 +1605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1621,7 +1628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1644,7 +1651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1667,7 +1674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1690,7 +1697,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1712,8 +1719,11 @@
       <c r="J14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -1735,8 +1745,11 @@
       <c r="J15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1758,8 +1771,11 @@
       <c r="J16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1781,8 +1797,11 @@
       <c r="J17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1804,8 +1823,11 @@
       <c r="J18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -1827,8 +1849,11 @@
       <c r="J19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -1850,8 +1875,11 @@
       <c r="J20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1873,8 +1901,11 @@
       <c r="J21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -1896,8 +1927,11 @@
       <c r="J22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -1919,8 +1953,11 @@
       <c r="J23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -1942,8 +1979,11 @@
       <c r="J24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -1965,8 +2005,11 @@
       <c r="J25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -1988,8 +2031,11 @@
       <c r="J26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -2011,8 +2057,11 @@
       <c r="J27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -2034,8 +2083,11 @@
       <c r="J28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -2057,8 +2109,11 @@
       <c r="J29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -2080,8 +2135,11 @@
       <c r="J30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -2103,8 +2161,11 @@
       <c r="J31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -2126,8 +2187,11 @@
       <c r="J32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -2149,8 +2213,11 @@
       <c r="J33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>99</v>
       </c>
@@ -2172,8 +2239,11 @@
       <c r="J34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -2195,8 +2265,11 @@
       <c r="J35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>105</v>
       </c>
@@ -2218,8 +2291,11 @@
       <c r="J36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>107</v>
       </c>
@@ -2241,8 +2317,11 @@
       <c r="J37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L37">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>110</v>
       </c>
@@ -2264,8 +2343,11 @@
       <c r="J38">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L38">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>111</v>
       </c>
@@ -2287,8 +2369,11 @@
       <c r="I39" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>114</v>
       </c>
@@ -2310,8 +2395,11 @@
       <c r="I40" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L40">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>116</v>
       </c>
@@ -2333,8 +2421,11 @@
       <c r="I41" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>118</v>
       </c>
@@ -2356,8 +2447,11 @@
       <c r="I42" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>120</v>
       </c>
@@ -2379,8 +2473,11 @@
       <c r="I43" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -2402,8 +2499,11 @@
       <c r="I44" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L44">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>124</v>
       </c>
@@ -2425,8 +2525,11 @@
       <c r="I45" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>126</v>
       </c>
@@ -2448,8 +2551,11 @@
       <c r="I46" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>128</v>
       </c>
@@ -2471,8 +2577,11 @@
       <c r="I47" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L47">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>130</v>
       </c>
@@ -2494,8 +2603,11 @@
       <c r="I48" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>132</v>
       </c>
@@ -2517,8 +2629,11 @@
       <c r="I49" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>134</v>
       </c>
@@ -2540,8 +2655,11 @@
       <c r="I50" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L50">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>136</v>
       </c>
@@ -2563,8 +2681,11 @@
       <c r="I51" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L51">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>138</v>
       </c>
@@ -2586,8 +2707,11 @@
       <c r="I52" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L52">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>140</v>
       </c>
@@ -2609,8 +2733,11 @@
       <c r="I53" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>142</v>
       </c>
@@ -2632,8 +2759,11 @@
       <c r="I54" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>144</v>
       </c>
@@ -2655,8 +2785,11 @@
       <c r="I55" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>146</v>
       </c>
@@ -2678,8 +2811,11 @@
       <c r="I56" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>148</v>
       </c>
@@ -2701,8 +2837,11 @@
       <c r="I57" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>150</v>
       </c>
@@ -2724,8 +2863,11 @@
       <c r="I58" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L58">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>152</v>
       </c>
@@ -2747,8 +2889,11 @@
       <c r="I59" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L59">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>154</v>
       </c>
@@ -2770,8 +2915,11 @@
       <c r="I60" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L60">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>156</v>
       </c>
@@ -2793,8 +2941,11 @@
       <c r="I61" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L61">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>158</v>
       </c>
@@ -2816,8 +2967,11 @@
       <c r="I62" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L62">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>160</v>
       </c>
@@ -2839,8 +2993,11 @@
       <c r="I63" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L63">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>162</v>
       </c>
@@ -2865,8 +3022,11 @@
       <c r="H64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L64">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>165</v>
       </c>
@@ -2891,8 +3051,11 @@
       <c r="H65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L65">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>167</v>
       </c>
@@ -2917,8 +3080,11 @@
       <c r="H66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L66">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>169</v>
       </c>
@@ -2943,8 +3109,11 @@
       <c r="H67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L67">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>172</v>
       </c>
@@ -2969,8 +3138,11 @@
       <c r="H68">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L68">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>175</v>
       </c>
@@ -2995,8 +3167,11 @@
       <c r="H69">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L69">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>177</v>
       </c>
@@ -3021,8 +3196,11 @@
       <c r="H70">
         <v>4</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L70">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>179</v>
       </c>
@@ -3047,8 +3225,11 @@
       <c r="H71">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L71">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>181</v>
       </c>
@@ -3073,8 +3254,11 @@
       <c r="H72">
         <v>5</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L72">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>183</v>
       </c>
@@ -3099,8 +3283,11 @@
       <c r="H73">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L73">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>186</v>
       </c>
@@ -3125,8 +3312,11 @@
       <c r="H74">
         <v>6</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L74">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>189</v>
       </c>
@@ -3151,8 +3341,11 @@
       <c r="H75">
         <v>6</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L75">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>192</v>
       </c>
@@ -3177,8 +3370,11 @@
       <c r="H76">
         <v>7</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L76">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>194</v>
       </c>
@@ -3203,8 +3399,11 @@
       <c r="H77">
         <v>7</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L77">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>197</v>
       </c>
@@ -3229,8 +3428,11 @@
       <c r="H78">
         <v>8</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L78">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>199</v>
       </c>
@@ -3255,8 +3457,11 @@
       <c r="H79">
         <v>8</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L79">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>202</v>
       </c>
@@ -3281,8 +3486,11 @@
       <c r="H80">
         <v>9</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L80">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>205</v>
       </c>
@@ -3307,8 +3515,11 @@
       <c r="H81">
         <v>9</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L81">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>208</v>
       </c>
@@ -3333,8 +3544,11 @@
       <c r="H82">
         <v>10</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L82">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>297</v>
       </c>
@@ -3359,8 +3573,11 @@
       <c r="H83">
         <v>10</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L83">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>210</v>
       </c>
@@ -3385,8 +3602,11 @@
       <c r="H84">
         <v>11</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L84">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>212</v>
       </c>
@@ -3411,8 +3631,11 @@
       <c r="H85">
         <v>11</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L85">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>214</v>
       </c>
@@ -3437,8 +3660,11 @@
       <c r="H86">
         <v>12</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L86">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>216</v>
       </c>
@@ -3463,8 +3689,11 @@
       <c r="H87">
         <v>12</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L87">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>219</v>
       </c>
@@ -3489,8 +3718,11 @@
       <c r="H88">
         <v>13</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L88">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>222</v>
       </c>
@@ -3515,8 +3747,11 @@
       <c r="H89">
         <v>13</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L89">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>224</v>
       </c>
@@ -3541,8 +3776,11 @@
       <c r="H90">
         <v>14</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L90">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>227</v>
       </c>
@@ -3567,8 +3805,11 @@
       <c r="H91">
         <v>14</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L91">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>231</v>
       </c>
@@ -3593,8 +3834,11 @@
       <c r="H92">
         <v>15</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L92">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>233</v>
       </c>
@@ -3619,8 +3863,11 @@
       <c r="H93">
         <v>15</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L93">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>236</v>
       </c>
@@ -3645,8 +3892,11 @@
       <c r="H94">
         <v>16</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L94">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>238</v>
       </c>
@@ -3671,8 +3921,11 @@
       <c r="H95">
         <v>16</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L95">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>241</v>
       </c>
@@ -3697,8 +3950,11 @@
       <c r="H96">
         <v>17</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L96">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>244</v>
       </c>
@@ -3723,8 +3979,11 @@
       <c r="H97">
         <v>17</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L97">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>246</v>
       </c>
@@ -3749,8 +4008,11 @@
       <c r="H98">
         <v>18</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L98">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>248</v>
       </c>
@@ -3775,8 +4037,11 @@
       <c r="H99">
         <v>18</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L99">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>250</v>
       </c>
@@ -3801,8 +4066,11 @@
       <c r="H100">
         <v>19</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L100">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>252</v>
       </c>
@@ -3827,8 +4095,11 @@
       <c r="H101">
         <v>19</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L101">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>254</v>
       </c>
@@ -3853,8 +4124,11 @@
       <c r="H102">
         <v>20</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L102">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>257</v>
       </c>
@@ -3878,6 +4152,9 @@
       </c>
       <c r="H103">
         <v>20</v>
+      </c>
+      <c r="L103">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the gears of corruption expansion
</commit_message>
<xml_diff>
--- a/scripts/cards.xlsx
+++ b/scripts/cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\navarog\projects\expeditions\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74ABC63-0B73-4C0D-BEBE-8B5553826666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731BD6E0-8CD2-446A-92F7-C9D6C1B14CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-83" yWindow="0" windowWidth="13905" windowHeight="13583" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="335">
   <si>
     <t>name</t>
   </si>
@@ -938,6 +938,93 @@
   </si>
   <si>
     <t>Control the Possessed</t>
+  </si>
+  <si>
+    <t>expansion</t>
+  </si>
+  <si>
+    <t>Bjorn</t>
+  </si>
+  <si>
+    <t>Gain a red worker OR Solve; if you Solve, gain the core value of all your solved quests.</t>
+  </si>
+  <si>
+    <t>gc</t>
+  </si>
+  <si>
+    <t>Mox</t>
+  </si>
+  <si>
+    <t>Play a card OR Vanquish; if this Vanquish removes the location's final corruption, you may gain the revealed benefit.</t>
+  </si>
+  <si>
+    <t>Freya</t>
+  </si>
+  <si>
+    <t>Sweep 1 face-up card to gain its core value OR Solve; if you Solve, gain the core value of all your solved quests.</t>
+  </si>
+  <si>
+    <t>Loki</t>
+  </si>
+  <si>
+    <t>Trash a card from the sweep pile to gain $1 OR Vanquish; if this Vanquish removes the location’s final corruption, you may gain the revealed benefit.</t>
+  </si>
+  <si>
+    <t>Zehra</t>
+  </si>
+  <si>
+    <t>Look at the top card of the deck and either return it to gain [Guile] or sweep it to gain [Power] OR Solve; if you Solve, gain the core value of all your solved quests.</t>
+  </si>
+  <si>
+    <t>Kar</t>
+  </si>
+  <si>
+    <t>Gain the top card of the deck OR Vanquish; if this Vanquish removes the location’s final corruption, you may gain the revealed benefit.</t>
+  </si>
+  <si>
+    <t>Baaliahon</t>
+  </si>
+  <si>
+    <t>Gain the top corruption accessible from your location (except the 20-value corruption token) OR pay [Guile][Power] to Meld.</t>
+  </si>
+  <si>
+    <t>Zephon</t>
+  </si>
+  <si>
+    <t>Activate a face-up purple card’s ability OR trash 1 corruption to tuck a quest.</t>
+  </si>
+  <si>
+    <t>Tesla Megacharger</t>
+  </si>
+  <si>
+    <t>Whenever you Upgrade another item, you may gain its instant benefit.</t>
+  </si>
+  <si>
+    <t>Sword of Nogai</t>
+  </si>
+  <si>
+    <t>Once per turn, if you rescue another card, you may gain a worker matching that card’s color.</t>
+  </si>
+  <si>
+    <t>The Eagle</t>
+  </si>
+  <si>
+    <t>Whenever you Solve, you may gain the Solved quest’s benefit twice (pay only once).</t>
+  </si>
+  <si>
+    <t>Ancient Wine</t>
+  </si>
+  <si>
+    <t>Whenever you gain a card, add it to your hand. Then each player gains [Power] or [Guile].</t>
+  </si>
+  <si>
+    <t>Gain [DrawCard]</t>
+  </si>
+  <si>
+    <t>Tainted Medallion</t>
+  </si>
+  <si>
+    <t>Whenever you Meld, you may play a card.</t>
   </si>
 </sst>
 </file>
@@ -991,10 +1078,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1057,9 +1147,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F42030B-66C5-46F6-8CFB-CD633B482508}" name="Table1" displayName="Table1" ref="A1:L103" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:L103" xr:uid="{0F42030B-66C5-46F6-8CFB-CD633B482508}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F42030B-66C5-46F6-8CFB-CD633B482508}" name="Table1" displayName="Table1" ref="A1:M116" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:M116" xr:uid="{0F42030B-66C5-46F6-8CFB-CD633B482508}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{C2006D74-3131-4AFC-AB17-9A5A423535C3}" name="name"/>
     <tableColumn id="2" xr3:uid="{3C4235A7-DBEF-42F6-B2B8-B558B520A439}" name="type"/>
     <tableColumn id="3" xr3:uid="{9445079D-106C-44A3-BE10-AD4E28465146}" name="ability"/>
@@ -1072,6 +1162,7 @@
     <tableColumn id="10" xr3:uid="{8BEE43DE-239D-482B-81BD-AA9B82DCD4C1}" name="coins"/>
     <tableColumn id="11" xr3:uid="{551EE5F0-3D63-4829-8E14-8064AD20AE34}" name="team"/>
     <tableColumn id="12" xr3:uid="{C1F323AB-632E-4110-88B0-57C52F4B4481}" name="number"/>
+    <tableColumn id="13" xr3:uid="{F37D05C1-203B-46D8-9EBD-5D229E388012}" name="expansion"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1362,28 +1453,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L103"/>
+  <dimension ref="A1:M116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="42.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="141.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="141.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.46484375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" customWidth="1"/>
-    <col min="9" max="9" width="41.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.86328125" customWidth="1"/>
+    <col min="9" max="9" width="41.46484375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.46484375" customWidth="1"/>
     <col min="11" max="11" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1420,8 +1511,11 @@
       <c r="L1" s="1" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1443,8 +1537,11 @@
       <c r="K2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1466,8 +1563,11 @@
       <c r="K3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1489,8 +1589,11 @@
       <c r="K4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1512,8 +1615,11 @@
       <c r="K5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1535,8 +1641,11 @@
       <c r="K6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1558,8 +1667,11 @@
       <c r="K7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1581,8 +1693,11 @@
       <c r="K8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1604,8 +1719,11 @@
       <c r="K9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1627,8 +1745,11 @@
       <c r="K10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1650,8 +1771,11 @@
       <c r="K11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1673,8 +1797,11 @@
       <c r="K12">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1696,8 +1823,11 @@
       <c r="K13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1722,8 +1852,11 @@
       <c r="L14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -1748,8 +1881,11 @@
       <c r="L15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1774,8 +1910,11 @@
       <c r="L16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1800,8 +1939,11 @@
       <c r="L17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1826,8 +1968,11 @@
       <c r="L18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -1852,8 +1997,11 @@
       <c r="L19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -1878,8 +2026,11 @@
       <c r="L20">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1904,8 +2055,11 @@
       <c r="L21">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -1930,8 +2084,11 @@
       <c r="L22">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -1956,8 +2113,11 @@
       <c r="L23">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -1974,16 +2134,19 @@
         <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>294</v>
+        <v>174</v>
       </c>
       <c r="J24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L24">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -2008,8 +2171,11 @@
       <c r="L25">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -2034,8 +2200,11 @@
       <c r="L26">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -2060,8 +2229,11 @@
       <c r="L27">
         <v>14</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -2086,8 +2258,11 @@
       <c r="L28">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -2112,8 +2287,11 @@
       <c r="L29">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -2138,8 +2316,11 @@
       <c r="L30">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -2164,8 +2345,11 @@
       <c r="L31">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -2190,8 +2374,11 @@
       <c r="L32">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -2216,8 +2403,11 @@
       <c r="L33">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>99</v>
       </c>
@@ -2242,8 +2432,11 @@
       <c r="L34">
         <v>21</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -2268,8 +2461,11 @@
       <c r="L35">
         <v>22</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>105</v>
       </c>
@@ -2294,8 +2490,11 @@
       <c r="L36">
         <v>23</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>107</v>
       </c>
@@ -2320,8 +2519,11 @@
       <c r="L37">
         <v>24</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>110</v>
       </c>
@@ -2346,8 +2548,11 @@
       <c r="L38">
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>111</v>
       </c>
@@ -2372,8 +2577,11 @@
       <c r="L39">
         <v>26</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>114</v>
       </c>
@@ -2398,8 +2606,11 @@
       <c r="L40">
         <v>27</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>116</v>
       </c>
@@ -2424,8 +2635,11 @@
       <c r="L41">
         <v>28</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>118</v>
       </c>
@@ -2450,8 +2664,11 @@
       <c r="L42">
         <v>29</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>120</v>
       </c>
@@ -2476,8 +2693,11 @@
       <c r="L43">
         <v>30</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -2502,8 +2722,11 @@
       <c r="L44">
         <v>31</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>124</v>
       </c>
@@ -2528,8 +2751,11 @@
       <c r="L45">
         <v>32</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>126</v>
       </c>
@@ -2554,8 +2780,11 @@
       <c r="L46">
         <v>33</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>128</v>
       </c>
@@ -2580,8 +2809,11 @@
       <c r="L47">
         <v>34</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>130</v>
       </c>
@@ -2606,8 +2838,11 @@
       <c r="L48">
         <v>35</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>132</v>
       </c>
@@ -2632,8 +2867,11 @@
       <c r="L49">
         <v>36</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>134</v>
       </c>
@@ -2658,8 +2896,11 @@
       <c r="L50">
         <v>37</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>136</v>
       </c>
@@ -2684,8 +2925,11 @@
       <c r="L51">
         <v>38</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>138</v>
       </c>
@@ -2710,8 +2954,11 @@
       <c r="L52">
         <v>39</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>140</v>
       </c>
@@ -2736,8 +2983,11 @@
       <c r="L53">
         <v>40</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>142</v>
       </c>
@@ -2762,8 +3012,11 @@
       <c r="L54">
         <v>41</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>144</v>
       </c>
@@ -2788,8 +3041,11 @@
       <c r="L55">
         <v>42</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>146</v>
       </c>
@@ -2814,8 +3070,11 @@
       <c r="L56">
         <v>43</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>148</v>
       </c>
@@ -2840,8 +3099,11 @@
       <c r="L57">
         <v>44</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>150</v>
       </c>
@@ -2866,8 +3128,11 @@
       <c r="L58">
         <v>45</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>152</v>
       </c>
@@ -2892,8 +3157,11 @@
       <c r="L59">
         <v>46</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M59" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>154</v>
       </c>
@@ -2918,8 +3186,11 @@
       <c r="L60">
         <v>47</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>156</v>
       </c>
@@ -2944,8 +3215,11 @@
       <c r="L61">
         <v>48</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>158</v>
       </c>
@@ -2970,8 +3244,11 @@
       <c r="L62">
         <v>49</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M62" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>160</v>
       </c>
@@ -2996,8 +3273,11 @@
       <c r="L63">
         <v>50</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M63" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>162</v>
       </c>
@@ -3025,8 +3305,11 @@
       <c r="L64">
         <v>51</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>165</v>
       </c>
@@ -3054,8 +3337,11 @@
       <c r="L65">
         <v>52</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>167</v>
       </c>
@@ -3083,8 +3369,11 @@
       <c r="L66">
         <v>53</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M66" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>169</v>
       </c>
@@ -3112,8 +3401,11 @@
       <c r="L67">
         <v>54</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>172</v>
       </c>
@@ -3141,8 +3433,11 @@
       <c r="L68">
         <v>55</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M68" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>175</v>
       </c>
@@ -3170,8 +3465,11 @@
       <c r="L69">
         <v>56</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M69" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>177</v>
       </c>
@@ -3199,8 +3497,11 @@
       <c r="L70">
         <v>57</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M70" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>179</v>
       </c>
@@ -3228,8 +3529,11 @@
       <c r="L71">
         <v>58</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>181</v>
       </c>
@@ -3257,8 +3561,11 @@
       <c r="L72">
         <v>59</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M72" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>183</v>
       </c>
@@ -3286,8 +3593,11 @@
       <c r="L73">
         <v>60</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>186</v>
       </c>
@@ -3315,8 +3625,11 @@
       <c r="L74">
         <v>61</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M74" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>189</v>
       </c>
@@ -3344,8 +3657,11 @@
       <c r="L75">
         <v>62</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>192</v>
       </c>
@@ -3373,8 +3689,11 @@
       <c r="L76">
         <v>63</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>194</v>
       </c>
@@ -3402,8 +3721,11 @@
       <c r="L77">
         <v>64</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>197</v>
       </c>
@@ -3431,8 +3753,11 @@
       <c r="L78">
         <v>65</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M78" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>199</v>
       </c>
@@ -3460,8 +3785,11 @@
       <c r="L79">
         <v>66</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M79" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>202</v>
       </c>
@@ -3489,8 +3817,11 @@
       <c r="L80">
         <v>67</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>205</v>
       </c>
@@ -3518,8 +3849,11 @@
       <c r="L81">
         <v>68</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M81" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>208</v>
       </c>
@@ -3547,8 +3881,11 @@
       <c r="L82">
         <v>69</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M82" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>296</v>
       </c>
@@ -3576,8 +3913,11 @@
       <c r="L83">
         <v>70</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M83" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>210</v>
       </c>
@@ -3605,8 +3945,11 @@
       <c r="L84">
         <v>71</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>212</v>
       </c>
@@ -3634,8 +3977,11 @@
       <c r="L85">
         <v>72</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M85" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>214</v>
       </c>
@@ -3663,8 +4009,11 @@
       <c r="L86">
         <v>73</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M86" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>216</v>
       </c>
@@ -3692,8 +4041,11 @@
       <c r="L87">
         <v>74</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M87" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>219</v>
       </c>
@@ -3721,8 +4073,11 @@
       <c r="L88">
         <v>75</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M88" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>222</v>
       </c>
@@ -3750,8 +4105,11 @@
       <c r="L89">
         <v>76</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M89" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>224</v>
       </c>
@@ -3779,8 +4137,11 @@
       <c r="L90">
         <v>77</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M90" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>227</v>
       </c>
@@ -3808,8 +4169,11 @@
       <c r="L91">
         <v>78</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>231</v>
       </c>
@@ -3837,8 +4201,11 @@
       <c r="L92">
         <v>79</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M92" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>233</v>
       </c>
@@ -3866,8 +4233,11 @@
       <c r="L93">
         <v>80</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M93" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>236</v>
       </c>
@@ -3895,8 +4265,11 @@
       <c r="L94">
         <v>81</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M94" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>238</v>
       </c>
@@ -3924,8 +4297,11 @@
       <c r="L95">
         <v>82</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M95" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>241</v>
       </c>
@@ -3953,8 +4329,11 @@
       <c r="L96">
         <v>83</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M96" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>244</v>
       </c>
@@ -3982,8 +4361,11 @@
       <c r="L97">
         <v>84</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M97" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>246</v>
       </c>
@@ -4011,8 +4393,11 @@
       <c r="L98">
         <v>85</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M98" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>248</v>
       </c>
@@ -4040,8 +4425,11 @@
       <c r="L99">
         <v>86</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M99" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>250</v>
       </c>
@@ -4069,8 +4457,11 @@
       <c r="L100">
         <v>87</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M100" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>252</v>
       </c>
@@ -4098,8 +4489,11 @@
       <c r="L101">
         <v>88</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M101" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>254</v>
       </c>
@@ -4127,8 +4521,11 @@
       <c r="L102">
         <v>89</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M102" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>305</v>
       </c>
@@ -4155,6 +4552,362 @@
       </c>
       <c r="L103">
         <v>90</v>
+      </c>
+      <c r="M103" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>307</v>
+      </c>
+      <c r="B104" t="s">
+        <v>12</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D104" t="s">
+        <v>20</v>
+      </c>
+      <c r="E104" t="s">
+        <v>15</v>
+      </c>
+      <c r="F104" t="s">
+        <v>16</v>
+      </c>
+      <c r="K104">
+        <v>7</v>
+      </c>
+      <c r="M104" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>310</v>
+      </c>
+      <c r="B105" t="s">
+        <v>18</v>
+      </c>
+      <c r="C105" t="s">
+        <v>311</v>
+      </c>
+      <c r="D105" t="s">
+        <v>31</v>
+      </c>
+      <c r="E105" t="s">
+        <v>21</v>
+      </c>
+      <c r="F105" t="s">
+        <v>40</v>
+      </c>
+      <c r="K105">
+        <v>7</v>
+      </c>
+      <c r="M105" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
+        <v>312</v>
+      </c>
+      <c r="B106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D106" t="s">
+        <v>25</v>
+      </c>
+      <c r="E106" t="s">
+        <v>15</v>
+      </c>
+      <c r="F106" t="s">
+        <v>22</v>
+      </c>
+      <c r="K106">
+        <v>10</v>
+      </c>
+      <c r="M106" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A107" t="s">
+        <v>314</v>
+      </c>
+      <c r="B107" t="s">
+        <v>18</v>
+      </c>
+      <c r="C107" t="s">
+        <v>315</v>
+      </c>
+      <c r="D107" t="s">
+        <v>31</v>
+      </c>
+      <c r="E107" t="s">
+        <v>21</v>
+      </c>
+      <c r="F107" t="s">
+        <v>16</v>
+      </c>
+      <c r="K107">
+        <v>10</v>
+      </c>
+      <c r="M107" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
+        <v>316</v>
+      </c>
+      <c r="B108" t="s">
+        <v>12</v>
+      </c>
+      <c r="C108" t="s">
+        <v>317</v>
+      </c>
+      <c r="D108" t="s">
+        <v>14</v>
+      </c>
+      <c r="E108" t="s">
+        <v>21</v>
+      </c>
+      <c r="F108" t="s">
+        <v>16</v>
+      </c>
+      <c r="K108">
+        <v>8</v>
+      </c>
+      <c r="M108" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
+        <v>318</v>
+      </c>
+      <c r="B109" t="s">
+        <v>18</v>
+      </c>
+      <c r="C109" t="s">
+        <v>319</v>
+      </c>
+      <c r="D109" t="s">
+        <v>25</v>
+      </c>
+      <c r="E109" t="s">
+        <v>21</v>
+      </c>
+      <c r="F109" t="s">
+        <v>26</v>
+      </c>
+      <c r="K109">
+        <v>8</v>
+      </c>
+      <c r="M109" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A110" t="s">
+        <v>320</v>
+      </c>
+      <c r="B110" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110" t="s">
+        <v>321</v>
+      </c>
+      <c r="D110" t="s">
+        <v>101</v>
+      </c>
+      <c r="E110" t="s">
+        <v>21</v>
+      </c>
+      <c r="F110" t="s">
+        <v>26</v>
+      </c>
+      <c r="K110">
+        <v>9</v>
+      </c>
+      <c r="M110" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A111" t="s">
+        <v>322</v>
+      </c>
+      <c r="B111" t="s">
+        <v>18</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D111" t="s">
+        <v>101</v>
+      </c>
+      <c r="E111" t="s">
+        <v>15</v>
+      </c>
+      <c r="F111" t="s">
+        <v>26</v>
+      </c>
+      <c r="K111">
+        <v>9</v>
+      </c>
+      <c r="M111" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A112" t="s">
+        <v>324</v>
+      </c>
+      <c r="B112" t="s">
+        <v>48</v>
+      </c>
+      <c r="C112" t="s">
+        <v>325</v>
+      </c>
+      <c r="D112" t="s">
+        <v>20</v>
+      </c>
+      <c r="E112" t="s">
+        <v>21</v>
+      </c>
+      <c r="G112" t="s">
+        <v>57</v>
+      </c>
+      <c r="J112">
+        <v>5</v>
+      </c>
+      <c r="L112">
+        <v>91</v>
+      </c>
+      <c r="M112" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A113" t="s">
+        <v>326</v>
+      </c>
+      <c r="B113" t="s">
+        <v>48</v>
+      </c>
+      <c r="C113" t="s">
+        <v>327</v>
+      </c>
+      <c r="D113" t="s">
+        <v>31</v>
+      </c>
+      <c r="E113" t="s">
+        <v>15</v>
+      </c>
+      <c r="G113" t="s">
+        <v>294</v>
+      </c>
+      <c r="J113">
+        <v>5</v>
+      </c>
+      <c r="L113">
+        <v>92</v>
+      </c>
+      <c r="M113" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A114" t="s">
+        <v>328</v>
+      </c>
+      <c r="B114" t="s">
+        <v>48</v>
+      </c>
+      <c r="C114" t="s">
+        <v>329</v>
+      </c>
+      <c r="D114" t="s">
+        <v>25</v>
+      </c>
+      <c r="E114" t="s">
+        <v>21</v>
+      </c>
+      <c r="G114" t="s">
+        <v>96</v>
+      </c>
+      <c r="J114">
+        <v>5</v>
+      </c>
+      <c r="L114">
+        <v>93</v>
+      </c>
+      <c r="M114" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A115" t="s">
+        <v>330</v>
+      </c>
+      <c r="B115" t="s">
+        <v>48</v>
+      </c>
+      <c r="C115" t="s">
+        <v>331</v>
+      </c>
+      <c r="D115" t="s">
+        <v>14</v>
+      </c>
+      <c r="E115" t="s">
+        <v>21</v>
+      </c>
+      <c r="G115" t="s">
+        <v>332</v>
+      </c>
+      <c r="J115">
+        <v>5</v>
+      </c>
+      <c r="L115">
+        <v>94</v>
+      </c>
+      <c r="M115" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A116" t="s">
+        <v>333</v>
+      </c>
+      <c r="B116" t="s">
+        <v>48</v>
+      </c>
+      <c r="C116" t="s">
+        <v>334</v>
+      </c>
+      <c r="D116" t="s">
+        <v>101</v>
+      </c>
+      <c r="E116" t="s">
+        <v>15</v>
+      </c>
+      <c r="G116" t="s">
+        <v>109</v>
+      </c>
+      <c r="J116">
+        <v>5</v>
+      </c>
+      <c r="L116">
+        <v>95</v>
+      </c>
+      <c r="M116" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>